<commit_message>
feat: added additional columns, expressions
</commit_message>
<xml_diff>
--- a/files/imdhub-site.xlsx
+++ b/files/imdhub-site.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="482">
   <si>
     <t>tableName</t>
   </si>
@@ -127,6 +127,18 @@
     <t>has given informed consent</t>
   </si>
   <si>
+    <t>has agreed to blood sampling</t>
+  </si>
+  <si>
+    <t>has agreed to urine sampling</t>
+  </si>
+  <si>
+    <t>has agreed to fibroblast sampling</t>
+  </si>
+  <si>
+    <t>has agreed to stool sampling</t>
+  </si>
+  <si>
     <t>has agreed to future reuse</t>
   </si>
   <si>
@@ -226,9 +238,6 @@
     <t>clinical metadata</t>
   </si>
   <si>
-    <t>clinical metadata transfered</t>
-  </si>
-  <si>
     <t>clinical metadata completeness</t>
   </si>
   <si>
@@ -460,6 +469,18 @@
     <t>Informed consent given</t>
   </si>
   <si>
+    <t>Does the participant agree to the donation of blood samples?</t>
+  </si>
+  <si>
+    <t>Does the participant agree to the donation of urine samples?</t>
+  </si>
+  <si>
+    <t>Does the participant agree to the donation of fibroblast samples?</t>
+  </si>
+  <si>
+    <t>Does the participant agree to the donation of stool samples?</t>
+  </si>
+  <si>
     <t>Does the participant agree to let us keep their data and samples in a permanent archive for future research related to IMD?</t>
   </si>
   <si>
@@ -472,7 +493,7 @@
     <t>Does the participant agree with the use of their samples for genetic testing?</t>
   </si>
   <si>
-    <t>Does the participant agree to take part in this study involving genetic analysis, which includes analysis of their genetic data?</t>
+    <t>Does the participant agree to take part in genetic analysis?</t>
   </si>
   <si>
     <t>Does the participant agree to allow the transfer of previously generated genetic data to researchers of the study for genetic analysis?</t>
@@ -545,15 +566,9 @@
     <t>Clinical metadata</t>
   </si>
   <si>
-    <t>Clinical metadata transferred</t>
-  </si>
-  <si>
     <t>Completeness of clinical metadata</t>
   </si>
   <si>
-    <t>Additional comments</t>
-  </si>
-  <si>
     <t>Enter the biospecimen identifier printed on the barcode</t>
   </si>
   <si>
@@ -722,16 +737,16 @@
     <t xml:space="preserve">Select the participant's cohort assignment </t>
   </si>
   <si>
-    <t xml:space="preserve">participants or legal representatives give written informed consent to study participation and consent for the collection and analysis of both blood and urine samples, and where indicated, a fibroblast sample or a stool sample. </t>
+    <t xml:space="preserve">Participants or legal representatives give written informed consent to study participation and consent for the collection and analysis of both blood and urine samples, and where indicated, a fibroblast sample or a stool sample. </t>
   </si>
   <si>
     <t>Participant is suspected to have an IMD and was advised on genetic testing.</t>
   </si>
   <si>
-    <t>Particpant is  informed of all the risks and benefits.</t>
-  </si>
-  <si>
-    <t>participants enrolled or registered with one of the following participant registries or cohort study (with ethical approval at site): U-IMD, GENOMIT or Solve-RD.</t>
+    <t>Particpant is informed of all the risks and benefits.</t>
+  </si>
+  <si>
+    <t>Participants enrolled or registered with one of the following participant registries or cohort study (with ethical approval at site): U-IMD, GENOMIT or Solve-RD.</t>
   </si>
   <si>
     <t>If the participant is part of a participant registry or cohort study, select the registry.</t>
@@ -746,7 +761,7 @@
     <t>E.g., HIV, infectious hepatitis, tuberculposis, or Creutzfeldt-Jakob disease</t>
   </si>
   <si>
-    <t>participant had a blood transfusion within the last month</t>
+    <t>Participant had a blood transfusion within the last month</t>
   </si>
   <si>
     <t>An indication that the participant meets selection criteria</t>
@@ -851,6 +866,18 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
   </si>
   <si>
+    <t>http://snomed.info/id/119297000</t>
+  </si>
+  <si>
+    <t>http://snomed.info/id/122575003</t>
+  </si>
+  <si>
+    <t>http://snomed.info/id/119333000</t>
+  </si>
+  <si>
+    <t>http://snomed.info/id/119339001</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/ICO_0000305</t>
   </si>
   <si>
@@ -932,15 +959,9 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C142478</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C95345</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/T4FS_0000191</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
   </si>
   <si>
@@ -1163,6 +1184,18 @@
     <t>if (hasGivenInformedConsent === null) "Indicate if the participant has given informed consent"</t>
   </si>
   <si>
+    <t>if (hasAgreedToBloodSampling === null) "Indicate if the participant agrees to blood sampling"</t>
+  </si>
+  <si>
+    <t>if (hasAgreedToUrineSampling === null) "Indicate if the participant agrees to urine sampling"</t>
+  </si>
+  <si>
+    <t>if (hasAgreedToFibroblastSampling === null) "Indicate if the participant agrees to fibroblast sampling"</t>
+  </si>
+  <si>
+    <t>if (hasAgreedToStoolSampling === null) "Indicate if the participant agrees to stool sampling"</t>
+  </si>
+  <si>
     <t>if (hasAgreedToFutureReuse === null) "Indicate if the participant has consented to future reuse"</t>
   </si>
   <si>
@@ -1175,16 +1208,16 @@
     <t>if (cohortAssignment.name === "Test cohort" &amp;&amp; hasAgreedToGeneticTesting == null) "Indicate if the participant has agreed to genetic testing"</t>
   </si>
   <si>
-    <t>if (hasAgreedToGeneticAnalysis === null) "Indicate if the participant has agreed to genetic analysis"</t>
-  </si>
-  <si>
-    <t>if (hasAgreedToTransferOfGeneticData === null) "Indicate if the participant has agreed to the transfer of genetic data"</t>
-  </si>
-  <si>
-    <t>if (hasAgreedToRecontactOfMedicalFindings === null) "Indicate if the participant has agreed to recontact in the event of medical findings"</t>
-  </si>
-  <si>
-    <t>if (hasAgreedToRecontactOfIncidentalFindings === null) "Indicate if the participant has agreed to recontact in the event of incidental findings"</t>
+    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToGeneticAnalysis === null ? "Indicate if the participant has agreed to genetic analysis" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToTransferOfGeneticData === null ? "Indicate if the participant has agreed to the transfer of genetic data" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToRecontactOfMedicalFindings === null ? "Indicate if the participant has agreed to recontact in the event of medical findings" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToRecontactOfIncidentalFindings === null ? "Indicate if the participant has agreed to recontact in the event of incidental findings" : false ) : false</t>
   </si>
   <si>
     <t>if (hasRegistryAffiliation === null) "Indicate if the participant is part of an existing registry, cohort, or study"</t>
@@ -1421,6 +1454,9 @@
   </si>
   <si>
     <t>cohortAssignment !== null ? (cohortAssignment.name === "Test cohort" ? true : false) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? !cohortAssignment.name.includes("Negative") : false</t>
   </si>
   <si>
     <t>hasRegistryAffiliation</t>
@@ -1862,7 +1898,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q113"/>
+  <dimension ref="A1:Q115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1926,16 +1962,16 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="P2" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q2" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1946,13 +1982,13 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="P3" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q3" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1963,31 +1999,31 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="H4" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="J4" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="L4" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="P4" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q4" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1998,28 +2034,28 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="I5" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J5" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="L5" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="P5" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q5" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2030,25 +2066,25 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E6" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="L6" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="P6" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q6" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2059,25 +2095,25 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="L7" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="O7" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="P7" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q7" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2088,28 +2124,28 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="I8" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J8" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="L8" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="P8" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q8" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2120,28 +2156,28 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="I9" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J9" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="L9" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="P9" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q9" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2152,19 +2188,19 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="P10" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q10" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2175,31 +2211,31 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="I11" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J11" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="L11" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="P11" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q11" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2210,19 +2246,19 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P12" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q12" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2233,25 +2269,25 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="L13" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="P13" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q13" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2262,22 +2298,22 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="L14" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="P14" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q14" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2288,31 +2324,22 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="I15" t="s">
-        <v>356</v>
-      </c>
-      <c r="J15" t="s">
-        <v>362</v>
+        <v>284</v>
       </c>
       <c r="L15" t="s">
-        <v>383</v>
-      </c>
-      <c r="M15" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
       <c r="P15" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q15" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2323,22 +2350,22 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="L16" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="P16" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q16" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2349,28 +2376,22 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" t="s">
-        <v>236</v>
+        <v>154</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="L17" t="s">
-        <v>385</v>
-      </c>
-      <c r="M17" t="s">
-        <v>444</v>
+        <v>392</v>
       </c>
       <c r="P17" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q17" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2381,25 +2402,22 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" t="s">
-        <v>237</v>
+        <v>155</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="L18" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="P18" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q18" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2413,19 +2431,28 @@
         <v>129</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
+      </c>
+      <c r="I19" t="s">
+        <v>363</v>
+      </c>
+      <c r="J19" t="s">
+        <v>369</v>
       </c>
       <c r="L19" t="s">
-        <v>387</v>
+        <v>394</v>
+      </c>
+      <c r="M19" t="s">
+        <v>454</v>
       </c>
       <c r="P19" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q19" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2436,22 +2463,22 @@
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="L20" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="P20" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q20" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2462,22 +2489,28 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
-        <v>155</v>
+        <v>158</v>
+      </c>
+      <c r="E21" t="s">
+        <v>241</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="L21" t="s">
-        <v>389</v>
+        <v>396</v>
+      </c>
+      <c r="M21" t="s">
+        <v>455</v>
       </c>
       <c r="P21" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q21" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2488,16 +2521,28 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="E22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L22" t="s">
+        <v>397</v>
+      </c>
+      <c r="M22" t="s">
+        <v>456</v>
       </c>
       <c r="P22" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q22" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2508,25 +2553,25 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
-        <v>157</v>
-      </c>
-      <c r="E23" t="s">
-        <v>238</v>
+        <v>160</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="L23" t="s">
-        <v>390</v>
+        <v>398</v>
+      </c>
+      <c r="M23" t="s">
+        <v>456</v>
       </c>
       <c r="P23" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q23" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2537,34 +2582,25 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
-      </c>
-      <c r="E24" t="s">
-        <v>239</v>
+        <v>161</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I24" t="s">
-        <v>356</v>
-      </c>
-      <c r="J24" t="s">
-        <v>363</v>
+        <v>291</v>
       </c>
       <c r="L24" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="M24" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="P24" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q24" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2575,25 +2611,25 @@
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="L25" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="M25" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="P25" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q25" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2604,16 +2640,16 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="P26" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q26" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2624,28 +2660,25 @@
         <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D27" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E27" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="L27" t="s">
-        <v>393</v>
-      </c>
-      <c r="M27" t="s">
-        <v>447</v>
+        <v>401</v>
       </c>
       <c r="P27" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q27" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2659,22 +2692,31 @@
         <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>244</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+      <c r="I28" t="s">
+        <v>363</v>
+      </c>
+      <c r="J28" t="s">
+        <v>370</v>
       </c>
       <c r="L28" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="M28" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="P28" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q28" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2685,25 +2727,25 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="L29" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="M29" t="s">
-        <v>447</v>
+        <v>458</v>
       </c>
       <c r="P29" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q29" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2714,28 +2756,16 @@
         <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" t="s">
-        <v>241</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="L30" t="s">
-        <v>396</v>
-      </c>
-      <c r="M30" t="s">
-        <v>447</v>
+        <v>167</v>
       </c>
       <c r="P30" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q30" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2746,28 +2776,28 @@
         <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="L31" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="M31" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="P31" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q31" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2778,28 +2808,25 @@
         <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
-      </c>
-      <c r="E32" t="s">
-        <v>243</v>
+        <v>169</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="L32" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="M32" t="s">
-        <v>445</v>
+        <v>459</v>
       </c>
       <c r="P32" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q32" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2810,22 +2837,25 @@
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="L33" t="s">
-        <v>399</v>
+        <v>406</v>
+      </c>
+      <c r="M33" t="s">
+        <v>459</v>
       </c>
       <c r="P33" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q33" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2836,25 +2866,28 @@
         <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>171</v>
+      </c>
+      <c r="E34" t="s">
+        <v>246</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="L34" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="M34" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
       <c r="P34" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q34" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2865,19 +2898,28 @@
         <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>172</v>
+      </c>
+      <c r="E35" t="s">
+        <v>247</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>294</v>
+        <v>299</v>
+      </c>
+      <c r="L35" t="s">
+        <v>408</v>
+      </c>
+      <c r="M35" t="s">
+        <v>459</v>
       </c>
       <c r="P35" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q35" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2888,25 +2930,28 @@
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="D36" t="s">
+        <v>173</v>
       </c>
       <c r="E36" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="G36" t="s">
-        <v>354</v>
+        <v>300</v>
+      </c>
+      <c r="L36" t="s">
+        <v>409</v>
       </c>
       <c r="M36" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="P36" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q36" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -2917,167 +2962,146 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" t="s">
-        <v>245</v>
+        <v>132</v>
+      </c>
+      <c r="D37" t="s">
+        <v>174</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="M37" t="s">
-        <v>450</v>
+        <v>301</v>
+      </c>
+      <c r="L37" t="s">
+        <v>410</v>
       </c>
       <c r="P37" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q37" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" t="s">
-        <v>246</v>
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" t="s">
+        <v>175</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
+      </c>
+      <c r="L38" t="s">
+        <v>411</v>
+      </c>
+      <c r="M38" t="s">
+        <v>460</v>
       </c>
       <c r="P38" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q38" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39" spans="1:17">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
-      </c>
-      <c r="E39" t="s">
-        <v>247</v>
+        <v>176</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="H39" t="s">
-        <v>355</v>
-      </c>
-      <c r="L39" t="s">
-        <v>401</v>
-      </c>
-      <c r="N39" t="s">
-        <v>465</v>
+        <v>303</v>
       </c>
       <c r="P39" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q39" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="40" spans="1:17">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="J40" t="s">
-        <v>17</v>
-      </c>
-      <c r="L40" t="s">
-        <v>402</v>
+        <v>304</v>
+      </c>
+      <c r="G40" t="s">
+        <v>361</v>
+      </c>
+      <c r="M40" t="s">
+        <v>461</v>
       </c>
       <c r="P40" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q40" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41" spans="1:17">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
-      </c>
-      <c r="D41" t="s">
-        <v>171</v>
+        <v>132</v>
+      </c>
+      <c r="E41" t="s">
+        <v>250</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="L41" t="s">
-        <v>403</v>
+        <v>305</v>
+      </c>
+      <c r="M41" t="s">
+        <v>462</v>
       </c>
       <c r="P41" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q41" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>18</v>
       </c>
-      <c r="B42" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" t="s">
-        <v>172</v>
-      </c>
       <c r="E42" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I42" t="s">
-        <v>356</v>
-      </c>
-      <c r="J42" t="s">
-        <v>364</v>
-      </c>
-      <c r="L42" t="s">
-        <v>404</v>
+        <v>306</v>
       </c>
       <c r="P42" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q42" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3088,25 +3112,31 @@
         <v>65</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E43" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>301</v>
+        <v>307</v>
+      </c>
+      <c r="H43" t="s">
+        <v>362</v>
       </c>
       <c r="L43" t="s">
-        <v>405</v>
+        <v>412</v>
+      </c>
+      <c r="N43" t="s">
+        <v>477</v>
       </c>
       <c r="P43" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q43" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3117,22 +3147,28 @@
         <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
-        <v>174</v>
+        <v>142</v>
+      </c>
+      <c r="E44" t="s">
+        <v>253</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>302</v>
+        <v>273</v>
+      </c>
+      <c r="J44" t="s">
+        <v>17</v>
       </c>
       <c r="L44" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="P44" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q44" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3143,16 +3179,22 @@
         <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="D45" t="s">
+        <v>178</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
+      </c>
+      <c r="L45" t="s">
+        <v>414</v>
       </c>
       <c r="P45" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q45" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -3163,22 +3205,31 @@
         <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>179</v>
+      </c>
+      <c r="E46" t="s">
+        <v>254</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>267</v>
+        <v>309</v>
+      </c>
+      <c r="I46" t="s">
+        <v>363</v>
       </c>
       <c r="J46" t="s">
-        <v>19</v>
-      </c>
-      <c r="K46" t="s">
-        <v>74</v>
+        <v>371</v>
+      </c>
+      <c r="L46" t="s">
+        <v>415</v>
       </c>
       <c r="P46" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q46" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -3189,22 +3240,25 @@
         <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E47" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>304</v>
+        <v>310</v>
+      </c>
+      <c r="L47" t="s">
+        <v>416</v>
       </c>
       <c r="P47" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q47" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -3215,19 +3269,22 @@
         <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>305</v>
+        <v>311</v>
+      </c>
+      <c r="L48" t="s">
+        <v>417</v>
       </c>
       <c r="P48" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q48" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -3240,17 +3297,14 @@
       <c r="C49" t="s">
         <v>134</v>
       </c>
-      <c r="D49" t="s">
-        <v>177</v>
-      </c>
       <c r="F49" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="P49" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q49" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3258,103 +3312,91 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
-      </c>
-      <c r="D50" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>307</v>
+        <v>272</v>
+      </c>
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" t="s">
+        <v>77</v>
       </c>
       <c r="P50" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q50" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" t="s">
+        <v>182</v>
       </c>
       <c r="E51" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>267</v>
+        <v>313</v>
       </c>
       <c r="P51" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q51" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D52" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="H52" t="s">
-        <v>355</v>
-      </c>
-      <c r="L52" t="s">
-        <v>407</v>
+        <v>314</v>
       </c>
       <c r="P52" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q52" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>19</v>
       </c>
-      <c r="B53" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" t="s">
-        <v>126</v>
-      </c>
-      <c r="D53" t="s">
-        <v>180</v>
-      </c>
       <c r="E53" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="I53" t="s">
-        <v>356</v>
-      </c>
-      <c r="J53" t="s">
-        <v>365</v>
-      </c>
-      <c r="L53" t="s">
-        <v>408</v>
+        <v>272</v>
       </c>
       <c r="P53" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q53" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -3362,28 +3404,28 @@
         <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="J54" t="s">
-        <v>18</v>
+        <v>272</v>
+      </c>
+      <c r="H54" t="s">
+        <v>362</v>
       </c>
       <c r="L54" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="P54" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q54" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -3391,25 +3433,34 @@
         <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
         <v>129</v>
       </c>
       <c r="D55" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="E55" t="s">
+        <v>258</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>310</v>
+        <v>315</v>
+      </c>
+      <c r="I55" t="s">
+        <v>363</v>
+      </c>
+      <c r="J55" t="s">
+        <v>372</v>
       </c>
       <c r="L55" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="P55" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q55" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -3417,28 +3468,28 @@
         <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
+      </c>
+      <c r="J56" t="s">
+        <v>18</v>
       </c>
       <c r="L56" t="s">
-        <v>411</v>
-      </c>
-      <c r="M56" t="s">
-        <v>451</v>
+        <v>420</v>
       </c>
       <c r="P56" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q56" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -3446,28 +3497,25 @@
         <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D57" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="L57" t="s">
-        <v>412</v>
-      </c>
-      <c r="M57" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="P57" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q57" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -3475,34 +3523,28 @@
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="I58" t="s">
-        <v>356</v>
-      </c>
-      <c r="J58" t="s">
-        <v>366</v>
+        <v>318</v>
       </c>
       <c r="L58" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="M58" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="P58" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q58" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -3510,31 +3552,28 @@
         <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D59" t="s">
-        <v>186</v>
-      </c>
-      <c r="E59" t="s">
-        <v>254</v>
+        <v>189</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="L59" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="M59" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="P59" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q59" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -3542,28 +3581,34 @@
         <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>312</v>
+        <v>320</v>
+      </c>
+      <c r="I60" t="s">
+        <v>363</v>
+      </c>
+      <c r="J60" t="s">
+        <v>373</v>
       </c>
       <c r="L60" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="M60" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="P60" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q60" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -3571,28 +3616,31 @@
         <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D61" t="s">
-        <v>188</v>
+        <v>191</v>
+      </c>
+      <c r="E61" t="s">
+        <v>259</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="L61" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="M61" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="P61" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q61" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -3600,25 +3648,28 @@
         <v>19</v>
       </c>
       <c r="B62" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>132</v>
+        <v>134</v>
+      </c>
+      <c r="D62" t="s">
+        <v>192</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="J62" t="s">
-        <v>20</v>
-      </c>
-      <c r="K62" t="s">
-        <v>88</v>
+        <v>319</v>
+      </c>
+      <c r="L62" t="s">
+        <v>426</v>
+      </c>
+      <c r="M62" t="s">
+        <v>466</v>
       </c>
       <c r="P62" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q62" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -3626,25 +3677,28 @@
         <v>19</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D63" t="s">
-        <v>189</v>
+        <v>193</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="L63" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="M63" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
       <c r="P63" t="s">
-        <v>469</v>
+        <v>361</v>
       </c>
       <c r="Q63" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -3652,31 +3706,25 @@
         <v>19</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
-        <v>126</v>
-      </c>
-      <c r="D64" t="s">
-        <v>190</v>
-      </c>
-      <c r="I64" t="s">
-        <v>356</v>
+        <v>135</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="J64" t="s">
-        <v>367</v>
-      </c>
-      <c r="L64" t="s">
-        <v>418</v>
-      </c>
-      <c r="M64" t="s">
-        <v>457</v>
+        <v>20</v>
+      </c>
+      <c r="K64" t="s">
+        <v>91</v>
       </c>
       <c r="P64" t="s">
-        <v>469</v>
+        <v>361</v>
       </c>
       <c r="Q64" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -3684,97 +3732,100 @@
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D65" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="L65" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="M65" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="P65" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="Q65" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" t="s">
-        <v>255</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>315</v>
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" t="s">
+        <v>129</v>
+      </c>
+      <c r="D66" t="s">
+        <v>195</v>
+      </c>
+      <c r="I66" t="s">
+        <v>363</v>
+      </c>
+      <c r="J66" t="s">
+        <v>374</v>
+      </c>
+      <c r="L66" t="s">
+        <v>429</v>
+      </c>
+      <c r="M66" t="s">
+        <v>469</v>
       </c>
       <c r="P66" t="s">
-        <v>354</v>
+        <v>481</v>
       </c>
       <c r="Q66" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="67" spans="1:17">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s">
-        <v>192</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H67" t="s">
-        <v>355</v>
-      </c>
-      <c r="N67" t="s">
-        <v>466</v>
+        <v>196</v>
+      </c>
+      <c r="L67" t="s">
+        <v>430</v>
+      </c>
+      <c r="M67" t="s">
+        <v>470</v>
       </c>
       <c r="P67" t="s">
-        <v>354</v>
+        <v>481</v>
       </c>
       <c r="Q67" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>20</v>
       </c>
-      <c r="B68" t="s">
-        <v>87</v>
-      </c>
-      <c r="C68" t="s">
-        <v>127</v>
-      </c>
-      <c r="D68" t="s">
-        <v>193</v>
+      <c r="E68" t="s">
+        <v>260</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L68" t="s">
-        <v>420</v>
+        <v>322</v>
       </c>
       <c r="P68" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q68" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -3782,28 +3833,28 @@
         <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D69" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="J69" t="s">
-        <v>19</v>
-      </c>
-      <c r="L69" t="s">
-        <v>421</v>
+        <v>323</v>
+      </c>
+      <c r="H69" t="s">
+        <v>362</v>
+      </c>
+      <c r="N69" t="s">
+        <v>478</v>
       </c>
       <c r="P69" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q69" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -3811,31 +3862,25 @@
         <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D70" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="I70" t="s">
-        <v>356</v>
-      </c>
-      <c r="J70" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="L70" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="P70" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q70" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -3843,22 +3888,28 @@
         <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D71" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>319</v>
+        <v>272</v>
+      </c>
+      <c r="J71" t="s">
+        <v>19</v>
+      </c>
+      <c r="L71" t="s">
+        <v>432</v>
       </c>
       <c r="P71" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q71" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="72" spans="1:17">
@@ -3866,22 +3917,31 @@
         <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D72" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
+      </c>
+      <c r="I72" t="s">
+        <v>363</v>
+      </c>
+      <c r="J72" t="s">
+        <v>374</v>
+      </c>
+      <c r="L72" t="s">
+        <v>433</v>
       </c>
       <c r="P72" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q72" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:17">
@@ -3889,22 +3949,22 @@
         <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D73" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="P73" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q73" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -3912,22 +3972,22 @@
         <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C74" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D74" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="P74" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q74" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -3935,22 +3995,22 @@
         <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C75" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="D75" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="P75" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q75" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -3958,31 +4018,22 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D76" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="I76" t="s">
-        <v>356</v>
-      </c>
-      <c r="J76" t="s">
-        <v>358</v>
-      </c>
-      <c r="L76" t="s">
-        <v>423</v>
+        <v>328</v>
       </c>
       <c r="P76" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q76" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -3990,31 +4041,22 @@
         <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D77" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="I77" t="s">
-        <v>356</v>
-      </c>
-      <c r="J77" t="s">
-        <v>358</v>
-      </c>
-      <c r="L77" t="s">
-        <v>424</v>
+        <v>329</v>
       </c>
       <c r="P77" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q77" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -4022,22 +4064,31 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C78" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D78" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>325</v>
+        <v>330</v>
+      </c>
+      <c r="I78" t="s">
+        <v>363</v>
+      </c>
+      <c r="J78" t="s">
+        <v>365</v>
+      </c>
+      <c r="L78" t="s">
+        <v>434</v>
       </c>
       <c r="P78" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q78" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -4045,22 +4096,31 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D79" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>326</v>
+        <v>331</v>
+      </c>
+      <c r="I79" t="s">
+        <v>363</v>
+      </c>
+      <c r="J79" t="s">
+        <v>365</v>
+      </c>
+      <c r="L79" t="s">
+        <v>435</v>
       </c>
       <c r="P79" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q79" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4068,97 +4128,85 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D80" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="P80" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q80" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="81" spans="1:17">
       <c r="A81" t="s">
-        <v>21</v>
-      </c>
-      <c r="E81" t="s">
-        <v>256</v>
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81" t="s">
+        <v>133</v>
+      </c>
+      <c r="D81" t="s">
+        <v>209</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="P81" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q81" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="82" spans="1:17">
       <c r="A82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C82" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D82" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="H82" t="s">
-        <v>355</v>
-      </c>
-      <c r="J82" t="s">
-        <v>17</v>
-      </c>
-      <c r="L82" t="s">
-        <v>425</v>
+        <v>334</v>
       </c>
       <c r="P82" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q82" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" spans="1:17">
       <c r="A83" t="s">
         <v>21</v>
       </c>
-      <c r="B83" t="s">
-        <v>99</v>
-      </c>
-      <c r="C83" t="s">
-        <v>129</v>
-      </c>
-      <c r="D83" t="s">
-        <v>207</v>
+      <c r="E83" t="s">
+        <v>261</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="L83" t="s">
-        <v>426</v>
+        <v>335</v>
       </c>
       <c r="P83" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q83" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -4166,34 +4214,31 @@
         <v>21</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="C84" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D84" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="I84" t="s">
-        <v>356</v>
+        <v>273</v>
+      </c>
+      <c r="H84" t="s">
+        <v>362</v>
       </c>
       <c r="J84" t="s">
-        <v>368</v>
+        <v>17</v>
       </c>
       <c r="L84" t="s">
-        <v>427</v>
-      </c>
-      <c r="M84" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="P84" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q84" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -4201,28 +4246,25 @@
         <v>21</v>
       </c>
       <c r="B85" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C85" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D85" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="L85" t="s">
-        <v>428</v>
-      </c>
-      <c r="M85" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="P85" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q85" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -4230,34 +4272,34 @@
         <v>21</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D86" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="I86" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J86" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="L86" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="M86" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P86" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q86" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="87" spans="1:17">
@@ -4265,28 +4307,28 @@
         <v>21</v>
       </c>
       <c r="B87" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C87" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="D87" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="L87" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="M87" t="s">
-        <v>459</v>
+        <v>472</v>
       </c>
       <c r="P87" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q87" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="1:17">
@@ -4294,34 +4336,34 @@
         <v>21</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C88" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D88" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="I88" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J88" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="L88" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="M88" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="P88" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q88" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -4329,28 +4371,28 @@
         <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C89" t="s">
         <v>130</v>
       </c>
       <c r="D89" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="L89" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="M89" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="P89" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q89" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:17">
@@ -4358,28 +4400,34 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
         <v>129</v>
       </c>
       <c r="D90" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>336</v>
+        <v>341</v>
+      </c>
+      <c r="I90" t="s">
+        <v>363</v>
+      </c>
+      <c r="J90" t="s">
+        <v>377</v>
       </c>
       <c r="L90" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="M90" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="P90" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q90" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -4387,103 +4435,103 @@
         <v>21</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C91" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D91" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="L91" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="M91" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="P91" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q91" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="92" spans="1:17">
       <c r="A92" t="s">
-        <v>22</v>
-      </c>
-      <c r="E92" t="s">
-        <v>257</v>
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>109</v>
+      </c>
+      <c r="C92" t="s">
+        <v>132</v>
+      </c>
+      <c r="D92" t="s">
+        <v>219</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>338</v>
+        <v>343</v>
+      </c>
+      <c r="L92" t="s">
+        <v>444</v>
+      </c>
+      <c r="M92" t="s">
+        <v>473</v>
       </c>
       <c r="P92" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q92" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:17">
       <c r="A93" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B93" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D93" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="H93" t="s">
-        <v>355</v>
-      </c>
-      <c r="J93" t="s">
-        <v>17</v>
+        <v>344</v>
       </c>
       <c r="L93" t="s">
-        <v>425</v>
+        <v>445</v>
+      </c>
+      <c r="M93" t="s">
+        <v>474</v>
       </c>
       <c r="P93" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q93" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="94" spans="1:17">
       <c r="A94" t="s">
         <v>22</v>
       </c>
-      <c r="B94" t="s">
-        <v>108</v>
-      </c>
-      <c r="C94" t="s">
-        <v>127</v>
-      </c>
-      <c r="D94" t="s">
-        <v>216</v>
+      <c r="E94" t="s">
+        <v>262</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="L94" t="s">
-        <v>435</v>
+        <v>345</v>
       </c>
       <c r="P94" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q94" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="95" spans="1:17">
@@ -4491,31 +4539,31 @@
         <v>22</v>
       </c>
       <c r="B95" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="C95" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D95" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="I95" t="s">
-        <v>356</v>
+        <v>273</v>
+      </c>
+      <c r="H95" t="s">
+        <v>362</v>
       </c>
       <c r="J95" t="s">
-        <v>371</v>
+        <v>17</v>
       </c>
       <c r="L95" t="s">
         <v>436</v>
       </c>
       <c r="P95" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q95" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:17">
@@ -4523,34 +4571,25 @@
         <v>22</v>
       </c>
       <c r="B96" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C96" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D96" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I96" t="s">
-        <v>356</v>
-      </c>
-      <c r="J96" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="L96" t="s">
-        <v>437</v>
-      </c>
-      <c r="M96" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="P96" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q96" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="97" spans="1:17">
@@ -4558,34 +4597,31 @@
         <v>22</v>
       </c>
       <c r="B97" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C97" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D97" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="I97" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J97" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="L97" t="s">
-        <v>438</v>
-      </c>
-      <c r="M97" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="P97" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q97" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="98" spans="1:17">
@@ -4593,106 +4629,115 @@
         <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C98" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D98" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>343</v>
+        <v>348</v>
+      </c>
+      <c r="I98" t="s">
+        <v>363</v>
+      </c>
+      <c r="J98" t="s">
+        <v>379</v>
       </c>
       <c r="L98" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="M98" t="s">
-        <v>464</v>
+        <v>475</v>
       </c>
       <c r="P98" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q98" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="99" spans="1:17">
       <c r="A99" t="s">
-        <v>23</v>
-      </c>
-      <c r="E99" t="s">
-        <v>258</v>
+        <v>22</v>
+      </c>
+      <c r="B99" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99" t="s">
+        <v>129</v>
+      </c>
+      <c r="D99" t="s">
+        <v>224</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>344</v>
+        <v>349</v>
+      </c>
+      <c r="I99" t="s">
+        <v>363</v>
+      </c>
+      <c r="J99" t="s">
+        <v>380</v>
+      </c>
+      <c r="L99" t="s">
+        <v>449</v>
+      </c>
+      <c r="M99" t="s">
+        <v>475</v>
       </c>
       <c r="P99" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q99" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="100" spans="1:17">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B100" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C100" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D100" t="s">
-        <v>221</v>
-      </c>
-      <c r="E100" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="J100" t="s">
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="L100" t="s">
-        <v>425</v>
+        <v>450</v>
+      </c>
+      <c r="M100" t="s">
+        <v>476</v>
       </c>
       <c r="P100" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q100" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="101" spans="1:17">
       <c r="A101" t="s">
         <v>23</v>
       </c>
-      <c r="B101" t="s">
-        <v>113</v>
-      </c>
-      <c r="C101" t="s">
-        <v>127</v>
-      </c>
-      <c r="D101" t="s">
-        <v>222</v>
-      </c>
       <c r="E101" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L101" t="s">
-        <v>440</v>
+        <v>351</v>
       </c>
       <c r="P101" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q101" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="102" spans="1:17">
@@ -4700,28 +4745,31 @@
         <v>23</v>
       </c>
       <c r="B102" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="C102" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D102" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E102" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>345</v>
+        <v>273</v>
+      </c>
+      <c r="J102" t="s">
+        <v>17</v>
       </c>
       <c r="L102" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="P102" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q102" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:17">
@@ -4729,28 +4777,28 @@
         <v>23</v>
       </c>
       <c r="B103" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C103" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D103" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E103" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="L103" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="P103" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q103" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="104" spans="1:17">
@@ -4758,25 +4806,28 @@
         <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C104" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D104" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E104" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>347</v>
+        <v>352</v>
+      </c>
+      <c r="L104" t="s">
+        <v>452</v>
       </c>
       <c r="P104" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q104" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:17">
@@ -4784,97 +4835,103 @@
         <v>23</v>
       </c>
       <c r="B105" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D105" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E105" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H105" t="s">
-        <v>355</v>
-      </c>
-      <c r="N105" t="s">
-        <v>467</v>
+        <v>353</v>
+      </c>
+      <c r="L105" t="s">
+        <v>453</v>
       </c>
       <c r="P105" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q105" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="106" spans="1:17">
       <c r="A106" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="B106" t="s">
+        <v>119</v>
+      </c>
+      <c r="C106" t="s">
+        <v>134</v>
+      </c>
+      <c r="D106" t="s">
+        <v>230</v>
       </c>
       <c r="E106" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="P106" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q106" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="107" spans="1:17">
       <c r="A107" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C107" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="D107" t="s">
-        <v>227</v>
+        <v>231</v>
+      </c>
+      <c r="E107" t="s">
+        <v>269</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>287</v>
+        <v>355</v>
       </c>
       <c r="H107" t="s">
-        <v>355</v>
+        <v>362</v>
+      </c>
+      <c r="N107" t="s">
+        <v>479</v>
       </c>
       <c r="P107" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q107" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="108" spans="1:17">
       <c r="A108" t="s">
         <v>24</v>
       </c>
-      <c r="B108" t="s">
-        <v>119</v>
-      </c>
-      <c r="C108" t="s">
-        <v>128</v>
-      </c>
-      <c r="D108" t="s">
-        <v>228</v>
+      <c r="E108" t="s">
+        <v>270</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="P108" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q108" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="109" spans="1:17">
@@ -4882,22 +4939,25 @@
         <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D109" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>351</v>
+        <v>296</v>
+      </c>
+      <c r="H109" t="s">
+        <v>362</v>
       </c>
       <c r="P109" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q109" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="110" spans="1:17">
@@ -4905,82 +4965,128 @@
         <v>24</v>
       </c>
       <c r="B110" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D110" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="P110" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q110" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="111" spans="1:17">
       <c r="A111" t="s">
-        <v>25</v>
-      </c>
-      <c r="E111" t="s">
-        <v>266</v>
+        <v>24</v>
+      </c>
+      <c r="B111" t="s">
+        <v>123</v>
+      </c>
+      <c r="C111" t="s">
+        <v>132</v>
+      </c>
+      <c r="D111" t="s">
+        <v>234</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="P111" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q111" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="1:17">
       <c r="A112" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C112" t="s">
-        <v>122</v>
+        <v>133</v>
+      </c>
+      <c r="D112" t="s">
+        <v>235</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="H112" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="P112" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q112" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="113" spans="1:17">
       <c r="A113" t="s">
         <v>25</v>
       </c>
-      <c r="B113" t="s">
-        <v>123</v>
-      </c>
-      <c r="C113" t="s">
-        <v>131</v>
+      <c r="E113" t="s">
+        <v>271</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c r="P113" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="Q113" t="s">
-        <v>354</v>
+        <v>361</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17">
+      <c r="A114" t="s">
+        <v>25</v>
+      </c>
+      <c r="B114" t="s">
+        <v>125</v>
+      </c>
+      <c r="C114" t="s">
+        <v>125</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="H114" t="s">
+        <v>362</v>
+      </c>
+      <c r="P114" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17">
+      <c r="A115" t="s">
+        <v>25</v>
+      </c>
+      <c r="B115" t="s">
+        <v>126</v>
+      </c>
+      <c r="C115" t="s">
+        <v>134</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="P115" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -5004,13 +5110,13 @@
     <hyperlink ref="F19" r:id="rId17"/>
     <hyperlink ref="F20" r:id="rId18"/>
     <hyperlink ref="F21" r:id="rId19"/>
-    <hyperlink ref="F23" r:id="rId20"/>
-    <hyperlink ref="F24" r:id="rId21"/>
-    <hyperlink ref="F25" r:id="rId22"/>
-    <hyperlink ref="F27" r:id="rId23"/>
-    <hyperlink ref="F28" r:id="rId24"/>
-    <hyperlink ref="F29" r:id="rId25"/>
-    <hyperlink ref="F30" r:id="rId26"/>
+    <hyperlink ref="F22" r:id="rId20"/>
+    <hyperlink ref="F23" r:id="rId21"/>
+    <hyperlink ref="F24" r:id="rId22"/>
+    <hyperlink ref="F25" r:id="rId23"/>
+    <hyperlink ref="F27" r:id="rId24"/>
+    <hyperlink ref="F28" r:id="rId25"/>
+    <hyperlink ref="F29" r:id="rId26"/>
     <hyperlink ref="F31" r:id="rId27"/>
     <hyperlink ref="F32" r:id="rId28"/>
     <hyperlink ref="F33" r:id="rId29"/>
@@ -5043,8 +5149,8 @@
     <hyperlink ref="F60" r:id="rId56"/>
     <hyperlink ref="F61" r:id="rId57"/>
     <hyperlink ref="F62" r:id="rId58"/>
-    <hyperlink ref="F66" r:id="rId59"/>
-    <hyperlink ref="F67" r:id="rId60"/>
+    <hyperlink ref="F63" r:id="rId59"/>
+    <hyperlink ref="F64" r:id="rId60"/>
     <hyperlink ref="F68" r:id="rId61"/>
     <hyperlink ref="F69" r:id="rId62"/>
     <hyperlink ref="F70" r:id="rId63"/>
@@ -5057,9 +5163,9 @@
     <hyperlink ref="F77" r:id="rId70"/>
     <hyperlink ref="F78" r:id="rId71"/>
     <hyperlink ref="F79" r:id="rId72"/>
-    <hyperlink ref="F80" r:id="rId73" location="comment"/>
+    <hyperlink ref="F80" r:id="rId73"/>
     <hyperlink ref="F81" r:id="rId74"/>
-    <hyperlink ref="F82" r:id="rId75"/>
+    <hyperlink ref="F82" r:id="rId75" location="comment"/>
     <hyperlink ref="F83" r:id="rId76"/>
     <hyperlink ref="F84" r:id="rId77"/>
     <hyperlink ref="F85" r:id="rId78"/>
@@ -5090,7 +5196,9 @@
     <hyperlink ref="F110" r:id="rId103"/>
     <hyperlink ref="F111" r:id="rId104"/>
     <hyperlink ref="F112" r:id="rId105"/>
-    <hyperlink ref="F113" r:id="rId106" location="comment"/>
+    <hyperlink ref="F113" r:id="rId106"/>
+    <hyperlink ref="F114" r:id="rId107"/>
+    <hyperlink ref="F115" r:id="rId108" location="comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: adjusted labels and description
</commit_message>
<xml_diff>
--- a/files/imdhub-site.xlsx
+++ b/files/imdhub-site.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="517">
   <si>
     <t>tableName</t>
   </si>
@@ -241,34 +241,10 @@
     <t>clinical metadata</t>
   </si>
   <si>
-    <t>demographics</t>
-  </si>
-  <si>
-    <t>partient status</t>
-  </si>
-  <si>
-    <t>disease history</t>
-  </si>
-  <si>
-    <t>medical history</t>
-  </si>
-  <si>
     <t>date clinical metadata received</t>
   </si>
   <si>
     <t>clinical metadata completeness</t>
-  </si>
-  <si>
-    <t>clinical exam</t>
-  </si>
-  <si>
-    <t>phenotypic features</t>
-  </si>
-  <si>
-    <t>treatment</t>
-  </si>
-  <si>
-    <t>lab analysis</t>
   </si>
   <si>
     <t>biospecimen id</t>
@@ -617,36 +593,12 @@
     <t>Clinical metadata</t>
   </si>
   <si>
-    <t>Demographic</t>
-  </si>
-  <si>
-    <t>Patient status</t>
-  </si>
-  <si>
-    <t>Disease history</t>
-  </si>
-  <si>
-    <t>Medical history</t>
-  </si>
-  <si>
     <t>Date clinical metadata received</t>
   </si>
   <si>
     <t>Completeness of clinical metadata</t>
   </si>
   <si>
-    <t>Clinical exam, body weight and height at time of visit</t>
-  </si>
-  <si>
-    <t>Disease signs and symptoms at time of visit</t>
-  </si>
-  <si>
-    <t>Treatment at time of visit</t>
-  </si>
-  <si>
-    <t>Laboratory analysis at time of visit</t>
-  </si>
-  <si>
     <t>Enter the biospecimen identifier printed on the barcode</t>
   </si>
   <si>
@@ -887,7 +839,7 @@
     <t xml:space="preserve">Fasting is when a subject doesn't eat or drink anything other than water only. </t>
   </si>
   <si>
-    <t>Demographics</t>
+    <t>Comprised of the following clinical data fields: Demographics, Patient status, Disease history [IMD diagnosis including primary mitochondrial disease (PMD), Metabolites at diagnosis, Genetic results], Medical history [Family IMD history, Other conditions], Clinical exam, body weight and height at time of visit, Disease signs and symptoms at time of visit [Clinical progression, Human Phenotype Ontology, Neuropsychological testing, PMD symptoms, PMD brain imaging results], Treatment at time of visit [Drug Treatment, Dietary treatment, Renal therapy, Non-pharmacologic therapies], Laboratory analysis at time of visit [ERKNet parameters, Metabolites at visit, PMD parameters]</t>
   </si>
   <si>
     <t>Biospecimen registrations by participant and visits</t>
@@ -2076,7 +2028,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q132"/>
+  <dimension ref="A1:Q124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2140,16 +2092,16 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="P2" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q2" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2160,13 +2112,13 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="P3" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q3" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2177,31 +2129,31 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E4" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="H4" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="J4" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="L4" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="P4" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q4" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2212,28 +2164,28 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="I5" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J5" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="L5" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="P5" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q5" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2244,25 +2196,25 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E6" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="L6" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="P6" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q6" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2273,25 +2225,25 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="L7" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="O7" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="P7" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q7" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2302,28 +2254,28 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="I8" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J8" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="L8" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="P8" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q8" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2334,28 +2286,28 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="I9" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J9" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="L9" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="P9" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q9" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2366,19 +2318,19 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="P10" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q10" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2389,31 +2341,31 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E11" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="I11" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J11" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="L11" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="P11" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q11" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2424,19 +2376,19 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="P12" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q12" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2447,25 +2399,25 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="L13" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="P13" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q13" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2476,22 +2428,22 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="L14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="P14" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q14" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2502,22 +2454,22 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="L15" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="P15" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q15" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2528,22 +2480,22 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="L16" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="P16" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q16" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2554,22 +2506,22 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="L17" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="P17" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q17" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2580,22 +2532,22 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="L18" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="P18" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q18" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2606,31 +2558,31 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="I19" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J19" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="L19" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="M19" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="P19" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q19" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2641,22 +2593,22 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="L20" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="P20" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q20" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2667,28 +2619,28 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E21" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="L21" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="M21" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="P21" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q21" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2699,28 +2651,28 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E22" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="L22" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="M22" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="P22" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q22" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2731,25 +2683,25 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="L23" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="M23" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="P23" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q23" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2760,25 +2712,25 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="L24" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="M24" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="P24" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q24" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2789,25 +2741,25 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="L25" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="M25" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="P25" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q25" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2818,16 +2770,16 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="P26" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q26" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2838,25 +2790,25 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="E27" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="L27" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="P27" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q27" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2867,34 +2819,34 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E28" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="I28" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J28" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="L28" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="M28" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="P28" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q28" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2905,25 +2857,25 @@
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="L29" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="M29" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="P29" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q29" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2934,16 +2886,16 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="P30" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q30" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2954,28 +2906,28 @@
         <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D31" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="E31" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="L31" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="M31" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="P31" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q31" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2986,25 +2938,25 @@
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="L32" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="M32" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="P32" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q32" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -3015,25 +2967,25 @@
         <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D33" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="L33" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="M33" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="P33" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q33" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -3044,28 +2996,28 @@
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D34" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="L34" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
       <c r="M34" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="P34" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q34" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -3076,28 +3028,28 @@
         <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D35" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="E35" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="L35" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="M35" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="P35" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q35" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -3108,28 +3060,28 @@
         <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D36" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E36" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="L36" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="M36" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="P36" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q36" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -3140,22 +3092,22 @@
         <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="L37" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="P37" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q37" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3166,25 +3118,25 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="L38" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="M38" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="P38" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q38" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -3195,19 +3147,19 @@
         <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="P39" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q39" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -3218,25 +3170,25 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E40" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="G40" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="M40" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="P40" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q40" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3247,22 +3199,22 @@
         <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E41" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="M41" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="P41" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q41" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -3270,16 +3222,16 @@
         <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="P42" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q42" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3290,31 +3242,31 @@
         <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D43" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E43" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="H43" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="L43" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="N43" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="P43" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q43" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3325,28 +3277,28 @@
         <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E44" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="J44" t="s">
         <v>17</v>
       </c>
       <c r="L44" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="P44" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q44" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3357,22 +3309,22 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="L45" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="P45" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q45" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -3383,31 +3335,31 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E46" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="I46" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J46" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="L46" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="P46" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q46" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -3418,25 +3370,25 @@
         <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E47" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="L47" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="P47" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q47" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -3447,22 +3399,22 @@
         <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="L48" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="P48" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q48" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -3473,16 +3425,16 @@
         <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="P49" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q49" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3493,22 +3445,22 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="J50" t="s">
         <v>19</v>
       </c>
       <c r="K50" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="P50" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q50" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -3519,22 +3471,22 @@
         <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D51" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E51" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="P51" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q51" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -3545,16 +3497,19 @@
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>200</v>
+        <v>192</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="P52" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q52" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -3565,199 +3520,277 @@
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="P53" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q53" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" t="s">
-        <v>144</v>
-      </c>
-      <c r="D54" t="s">
-        <v>202</v>
+        <v>19</v>
+      </c>
+      <c r="E54" t="s">
+        <v>275</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="P54" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q54" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s">
-        <v>203</v>
+        <v>194</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H55" t="s">
+        <v>390</v>
+      </c>
+      <c r="L55" t="s">
+        <v>446</v>
       </c>
       <c r="P55" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q55" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>204</v>
+        <v>195</v>
+      </c>
+      <c r="E56" t="s">
+        <v>276</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
+      </c>
+      <c r="I56" t="s">
+        <v>391</v>
+      </c>
+      <c r="J56" t="s">
+        <v>400</v>
+      </c>
+      <c r="L56" t="s">
+        <v>447</v>
       </c>
       <c r="P56" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q56" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="57" spans="1:17">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D57" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
+      </c>
+      <c r="M57" t="s">
+        <v>492</v>
+      </c>
+      <c r="N57" t="s">
+        <v>510</v>
+      </c>
+      <c r="O57" t="s">
+        <v>514</v>
       </c>
       <c r="P57" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q57" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="58" spans="1:17">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
-        <v>206</v>
+        <v>197</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="L58" t="s">
+        <v>448</v>
+      </c>
+      <c r="M58" t="s">
+        <v>493</v>
+      </c>
+      <c r="O58" t="s">
+        <v>515</v>
       </c>
       <c r="P58" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q58" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" t="s">
+        <v>198</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J59" t="s">
         <v>18</v>
       </c>
-      <c r="B59" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" t="s">
-        <v>153</v>
-      </c>
-      <c r="D59" t="s">
-        <v>207</v>
+      <c r="L59" t="s">
+        <v>449</v>
       </c>
       <c r="P59" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q59" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D60" t="s">
-        <v>208</v>
+        <v>199</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="L60" t="s">
+        <v>450</v>
       </c>
       <c r="P60" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q60" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D61" t="s">
-        <v>209</v>
+        <v>200</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="L61" t="s">
+        <v>451</v>
+      </c>
+      <c r="M61" t="s">
+        <v>494</v>
       </c>
       <c r="P61" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q61" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>19</v>
       </c>
-      <c r="E62" t="s">
-        <v>291</v>
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" t="s">
+        <v>201</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>306</v>
+        <v>340</v>
+      </c>
+      <c r="L62" t="s">
+        <v>452</v>
+      </c>
+      <c r="M62" t="s">
+        <v>495</v>
       </c>
       <c r="P62" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q62" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -3768,25 +3801,31 @@
         <v>85</v>
       </c>
       <c r="C63" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D63" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H63" t="s">
-        <v>406</v>
+        <v>341</v>
+      </c>
+      <c r="I63" t="s">
+        <v>391</v>
+      </c>
+      <c r="J63" t="s">
+        <v>401</v>
       </c>
       <c r="L63" t="s">
-        <v>462</v>
+        <v>453</v>
+      </c>
+      <c r="M63" t="s">
+        <v>496</v>
       </c>
       <c r="P63" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q63" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -3797,31 +3836,28 @@
         <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D64" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E64" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="I64" t="s">
-        <v>407</v>
-      </c>
-      <c r="J64" t="s">
-        <v>416</v>
+        <v>339</v>
       </c>
       <c r="L64" t="s">
-        <v>463</v>
+        <v>454</v>
+      </c>
+      <c r="M64" t="s">
+        <v>494</v>
       </c>
       <c r="P64" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q64" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -3832,28 +3868,25 @@
         <v>87</v>
       </c>
       <c r="C65" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D65" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>351</v>
+        <v>340</v>
+      </c>
+      <c r="L65" t="s">
+        <v>455</v>
       </c>
       <c r="M65" t="s">
-        <v>508</v>
-      </c>
-      <c r="N65" t="s">
-        <v>526</v>
-      </c>
-      <c r="O65" t="s">
-        <v>530</v>
+        <v>497</v>
       </c>
       <c r="P65" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q65" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="66" spans="1:17">
@@ -3864,28 +3897,25 @@
         <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D66" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="L66" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="M66" t="s">
-        <v>509</v>
-      </c>
-      <c r="O66" t="s">
-        <v>531</v>
+        <v>498</v>
       </c>
       <c r="P66" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q66" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -3896,25 +3926,22 @@
         <v>89</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
-      </c>
-      <c r="D67" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="J67" t="s">
-        <v>18</v>
-      </c>
-      <c r="L67" t="s">
-        <v>465</v>
+        <v>20</v>
+      </c>
+      <c r="K67" t="s">
+        <v>95</v>
       </c>
       <c r="P67" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q67" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -3925,22 +3952,25 @@
         <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D68" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="L68" t="s">
-        <v>466</v>
+        <v>457</v>
+      </c>
+      <c r="M68" t="s">
+        <v>499</v>
       </c>
       <c r="P68" t="s">
-        <v>405</v>
+        <v>516</v>
       </c>
       <c r="Q68" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -3951,25 +3981,31 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
+      </c>
+      <c r="I69" t="s">
+        <v>391</v>
+      </c>
+      <c r="J69" t="s">
+        <v>402</v>
       </c>
       <c r="L69" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="M69" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="P69" t="s">
-        <v>405</v>
+        <v>516</v>
       </c>
       <c r="Q69" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -3980,286 +4016,250 @@
         <v>92</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="L70" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="M70" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="P70" t="s">
-        <v>405</v>
+        <v>516</v>
       </c>
       <c r="Q70" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="1:17">
       <c r="A71" t="s">
-        <v>19</v>
-      </c>
-      <c r="B71" t="s">
-        <v>93</v>
-      </c>
-      <c r="C71" t="s">
-        <v>155</v>
-      </c>
-      <c r="D71" t="s">
-        <v>218</v>
+        <v>20</v>
+      </c>
+      <c r="E71" t="s">
+        <v>278</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="I71" t="s">
-        <v>407</v>
-      </c>
-      <c r="J71" t="s">
-        <v>417</v>
-      </c>
-      <c r="L71" t="s">
-        <v>469</v>
-      </c>
-      <c r="M71" t="s">
-        <v>512</v>
+        <v>343</v>
       </c>
       <c r="P71" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q71" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>219</v>
-      </c>
-      <c r="E72" t="s">
-        <v>293</v>
+        <v>209</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="L72" t="s">
-        <v>470</v>
-      </c>
-      <c r="M72" t="s">
-        <v>510</v>
+        <v>346</v>
+      </c>
+      <c r="H72" t="s">
+        <v>390</v>
+      </c>
+      <c r="N72" t="s">
+        <v>511</v>
       </c>
       <c r="P72" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q72" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="L73" t="s">
-        <v>471</v>
-      </c>
-      <c r="M73" t="s">
-        <v>513</v>
+        <v>460</v>
       </c>
       <c r="P73" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q73" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" t="s">
+        <v>149</v>
+      </c>
+      <c r="D74" t="s">
+        <v>211</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="J74" t="s">
         <v>19</v>
       </c>
-      <c r="B74" t="s">
-        <v>96</v>
-      </c>
-      <c r="C74" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" t="s">
-        <v>221</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="L74" t="s">
-        <v>472</v>
-      </c>
-      <c r="M74" t="s">
-        <v>514</v>
+        <v>461</v>
       </c>
       <c r="P74" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q74" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="75" spans="1:17">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>138</v>
+      </c>
+      <c r="D75" t="s">
+        <v>212</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>359</v>
+        <v>348</v>
+      </c>
+      <c r="I75" t="s">
+        <v>391</v>
       </c>
       <c r="J75" t="s">
-        <v>20</v>
-      </c>
-      <c r="K75" t="s">
-        <v>103</v>
+        <v>402</v>
+      </c>
+      <c r="L75" t="s">
+        <v>462</v>
       </c>
       <c r="P75" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q75" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="A76" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D76" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="L76" t="s">
-        <v>473</v>
-      </c>
-      <c r="M76" t="s">
-        <v>515</v>
+        <v>349</v>
       </c>
       <c r="P76" t="s">
-        <v>532</v>
+        <v>389</v>
       </c>
       <c r="Q76" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="77" spans="1:17">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C77" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D77" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="I77" t="s">
-        <v>407</v>
-      </c>
-      <c r="J77" t="s">
-        <v>418</v>
-      </c>
-      <c r="L77" t="s">
-        <v>474</v>
-      </c>
-      <c r="M77" t="s">
-        <v>516</v>
+        <v>350</v>
       </c>
       <c r="P77" t="s">
-        <v>532</v>
+        <v>389</v>
       </c>
       <c r="Q77" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="78" spans="1:17">
       <c r="A78" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D78" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="L78" t="s">
-        <v>475</v>
-      </c>
-      <c r="M78" t="s">
-        <v>517</v>
+        <v>350</v>
       </c>
       <c r="P78" t="s">
-        <v>532</v>
+        <v>389</v>
       </c>
       <c r="Q78" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>20</v>
       </c>
-      <c r="E79" t="s">
-        <v>294</v>
+      <c r="B79" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" t="s">
+        <v>142</v>
+      </c>
+      <c r="D79" t="s">
+        <v>216</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="P79" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q79" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4270,25 +4270,19 @@
         <v>101</v>
       </c>
       <c r="C80" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="D80" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="H80" t="s">
-        <v>406</v>
-      </c>
-      <c r="N80" t="s">
-        <v>527</v>
+        <v>352</v>
       </c>
       <c r="P80" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q80" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="81" spans="1:17">
@@ -4299,22 +4293,28 @@
         <v>102</v>
       </c>
       <c r="C81" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D81" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
+      </c>
+      <c r="I81" t="s">
+        <v>391</v>
+      </c>
+      <c r="J81" t="s">
+        <v>393</v>
       </c>
       <c r="L81" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="P81" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q81" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="82" spans="1:17">
@@ -4325,25 +4325,28 @@
         <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D82" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>306</v>
+        <v>354</v>
+      </c>
+      <c r="I82" t="s">
+        <v>391</v>
       </c>
       <c r="J82" t="s">
-        <v>19</v>
+        <v>393</v>
       </c>
       <c r="L82" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="P82" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q82" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -4354,28 +4357,19 @@
         <v>104</v>
       </c>
       <c r="C83" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D83" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="I83" t="s">
-        <v>407</v>
-      </c>
-      <c r="J83" t="s">
-        <v>418</v>
-      </c>
-      <c r="L83" t="s">
-        <v>478</v>
+        <v>355</v>
       </c>
       <c r="P83" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q83" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -4386,19 +4380,19 @@
         <v>105</v>
       </c>
       <c r="C84" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D84" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="P84" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q84" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -4406,241 +4400,292 @@
         <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C85" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D85" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="P85" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q85" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" t="s">
-        <v>107</v>
-      </c>
-      <c r="C86" t="s">
-        <v>158</v>
-      </c>
-      <c r="D86" t="s">
-        <v>231</v>
+        <v>21</v>
+      </c>
+      <c r="E86" t="s">
+        <v>279</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="P86" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q86" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="87" spans="1:17">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="C87" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D87" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>367</v>
+        <v>291</v>
+      </c>
+      <c r="H87" t="s">
+        <v>390</v>
+      </c>
+      <c r="J87" t="s">
+        <v>17</v>
+      </c>
+      <c r="L87" t="s">
+        <v>465</v>
       </c>
       <c r="P87" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q87" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="88" spans="1:17">
       <c r="A88" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C88" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D88" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>368</v>
+        <v>359</v>
+      </c>
+      <c r="L88" t="s">
+        <v>466</v>
+      </c>
+      <c r="M88" t="s">
+        <v>502</v>
       </c>
       <c r="P88" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q88" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="89" spans="1:17">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C89" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D89" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="I89" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="J89" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="L89" t="s">
-        <v>479</v>
+        <v>467</v>
+      </c>
+      <c r="M89" t="s">
+        <v>503</v>
       </c>
       <c r="P89" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q89" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="90" spans="1:17">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C90" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D90" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="I90" t="s">
-        <v>407</v>
-      </c>
-      <c r="J90" t="s">
-        <v>409</v>
+        <v>361</v>
       </c>
       <c r="L90" t="s">
-        <v>480</v>
+        <v>468</v>
+      </c>
+      <c r="M90" t="s">
+        <v>504</v>
       </c>
       <c r="P90" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q90" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="91" spans="1:17">
       <c r="A91" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D91" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>371</v>
+        <v>362</v>
+      </c>
+      <c r="I91" t="s">
+        <v>391</v>
+      </c>
+      <c r="J91" t="s">
+        <v>404</v>
+      </c>
+      <c r="L91" t="s">
+        <v>469</v>
+      </c>
+      <c r="M91" t="s">
+        <v>503</v>
       </c>
       <c r="P91" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q91" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="92" spans="1:17">
       <c r="A92" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D92" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>372</v>
+        <v>363</v>
+      </c>
+      <c r="L92" t="s">
+        <v>470</v>
+      </c>
+      <c r="M92" t="s">
+        <v>503</v>
       </c>
       <c r="P92" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q92" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="93" spans="1:17">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D93" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>373</v>
+        <v>364</v>
+      </c>
+      <c r="I93" t="s">
+        <v>391</v>
+      </c>
+      <c r="J93" t="s">
+        <v>405</v>
+      </c>
+      <c r="L93" t="s">
+        <v>471</v>
+      </c>
+      <c r="M93" t="s">
+        <v>503</v>
       </c>
       <c r="P93" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q93" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:17">
       <c r="A94" t="s">
         <v>21</v>
       </c>
-      <c r="E94" t="s">
-        <v>295</v>
+      <c r="B94" t="s">
+        <v>112</v>
+      </c>
+      <c r="C94" t="s">
+        <v>142</v>
+      </c>
+      <c r="D94" t="s">
+        <v>230</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>374</v>
+        <v>365</v>
+      </c>
+      <c r="L94" t="s">
+        <v>472</v>
+      </c>
+      <c r="M94" t="s">
+        <v>505</v>
       </c>
       <c r="P94" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q94" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="95" spans="1:17">
@@ -4648,31 +4693,28 @@
         <v>21</v>
       </c>
       <c r="B95" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D95" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="H95" t="s">
-        <v>406</v>
-      </c>
-      <c r="J95" t="s">
-        <v>17</v>
+        <v>366</v>
       </c>
       <c r="L95" t="s">
-        <v>481</v>
+        <v>473</v>
+      </c>
+      <c r="M95" t="s">
+        <v>505</v>
       </c>
       <c r="P95" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q95" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="96" spans="1:17">
@@ -4683,994 +4725,744 @@
         <v>114</v>
       </c>
       <c r="C96" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D96" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="L96" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="M96" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="P96" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q96" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="97" spans="1:17">
       <c r="A97" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B97" t="s">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="C97" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D97" t="s">
-        <v>241</v>
+        <v>233</v>
+      </c>
+      <c r="E97" t="s">
+        <v>271</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="I97" t="s">
-        <v>407</v>
+        <v>291</v>
+      </c>
+      <c r="H97" t="s">
+        <v>390</v>
       </c>
       <c r="J97" t="s">
-        <v>419</v>
-      </c>
-      <c r="L97" t="s">
-        <v>483</v>
-      </c>
-      <c r="M97" t="s">
-        <v>519</v>
+        <v>17</v>
       </c>
       <c r="P97" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q97" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="98" spans="1:17">
       <c r="A98" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C98" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D98" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="L98" t="s">
-        <v>484</v>
-      </c>
-      <c r="M98" t="s">
-        <v>520</v>
+        <v>368</v>
       </c>
       <c r="P98" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q98" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="99" spans="1:17">
       <c r="A99" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B99" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C99" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D99" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="I99" t="s">
-        <v>407</v>
-      </c>
-      <c r="J99" t="s">
-        <v>420</v>
-      </c>
-      <c r="L99" t="s">
-        <v>485</v>
-      </c>
-      <c r="M99" t="s">
-        <v>519</v>
+        <v>369</v>
       </c>
       <c r="P99" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q99" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="100" spans="1:17">
       <c r="A100" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B100" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C100" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D100" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="L100" t="s">
-        <v>486</v>
-      </c>
-      <c r="M100" t="s">
-        <v>519</v>
+        <v>370</v>
       </c>
       <c r="P100" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q100" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="101" spans="1:17">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B101" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D101" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="I101" t="s">
-        <v>407</v>
-      </c>
-      <c r="J101" t="s">
-        <v>421</v>
-      </c>
-      <c r="L101" t="s">
-        <v>487</v>
-      </c>
-      <c r="M101" t="s">
-        <v>519</v>
+        <v>371</v>
       </c>
       <c r="P101" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q101" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="102" spans="1:17">
       <c r="A102" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B102" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C102" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D102" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="L102" t="s">
-        <v>488</v>
-      </c>
-      <c r="M102" t="s">
-        <v>521</v>
+        <v>372</v>
       </c>
       <c r="P102" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q102" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="103" spans="1:17">
       <c r="A103" t="s">
-        <v>21</v>
-      </c>
-      <c r="B103" t="s">
-        <v>121</v>
-      </c>
-      <c r="C103" t="s">
-        <v>149</v>
-      </c>
-      <c r="D103" t="s">
-        <v>247</v>
+        <v>23</v>
+      </c>
+      <c r="E103" t="s">
+        <v>280</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="L103" t="s">
-        <v>489</v>
-      </c>
-      <c r="M103" t="s">
-        <v>521</v>
+        <v>373</v>
       </c>
       <c r="P103" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q103" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" spans="1:17">
       <c r="A104" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="C104" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D104" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>383</v>
+        <v>291</v>
+      </c>
+      <c r="H104" t="s">
+        <v>390</v>
+      </c>
+      <c r="J104" t="s">
+        <v>17</v>
       </c>
       <c r="L104" t="s">
-        <v>490</v>
-      </c>
-      <c r="M104" t="s">
-        <v>522</v>
+        <v>465</v>
       </c>
       <c r="P104" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q104" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="105" spans="1:17">
       <c r="A105" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B105" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="C105" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D105" t="s">
-        <v>249</v>
-      </c>
-      <c r="E105" t="s">
-        <v>287</v>
+        <v>239</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="H105" t="s">
-        <v>406</v>
-      </c>
-      <c r="J105" t="s">
-        <v>17</v>
+        <v>374</v>
+      </c>
+      <c r="L105" t="s">
+        <v>475</v>
       </c>
       <c r="P105" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q105" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="106" spans="1:17">
       <c r="A106" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B106" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C106" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D106" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>384</v>
+        <v>375</v>
+      </c>
+      <c r="I106" t="s">
+        <v>391</v>
+      </c>
+      <c r="J106" t="s">
+        <v>406</v>
+      </c>
+      <c r="L106" t="s">
+        <v>476</v>
       </c>
       <c r="P106" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q106" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="107" spans="1:17">
       <c r="A107" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D107" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>385</v>
+        <v>376</v>
+      </c>
+      <c r="I107" t="s">
+        <v>391</v>
+      </c>
+      <c r="J107" t="s">
+        <v>407</v>
+      </c>
+      <c r="L107" t="s">
+        <v>477</v>
+      </c>
+      <c r="M107" t="s">
+        <v>507</v>
       </c>
       <c r="P107" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q107" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="108" spans="1:17">
       <c r="A108" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B108" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C108" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D108" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>386</v>
+        <v>377</v>
+      </c>
+      <c r="I108" t="s">
+        <v>391</v>
+      </c>
+      <c r="J108" t="s">
+        <v>408</v>
+      </c>
+      <c r="L108" t="s">
+        <v>478</v>
+      </c>
+      <c r="M108" t="s">
+        <v>507</v>
       </c>
       <c r="P108" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q108" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="109" spans="1:17">
       <c r="A109" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B109" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C109" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D109" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>387</v>
+        <v>378</v>
+      </c>
+      <c r="L109" t="s">
+        <v>479</v>
+      </c>
+      <c r="M109" t="s">
+        <v>508</v>
       </c>
       <c r="P109" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q109" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="110" spans="1:17">
       <c r="A110" t="s">
-        <v>22</v>
-      </c>
-      <c r="B110" t="s">
-        <v>127</v>
-      </c>
-      <c r="C110" t="s">
-        <v>150</v>
-      </c>
-      <c r="D110" t="s">
-        <v>254</v>
+        <v>24</v>
+      </c>
+      <c r="E110" t="s">
+        <v>281</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="P110" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q110" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="111" spans="1:17">
       <c r="A111" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B111" t="s">
+        <v>67</v>
+      </c>
+      <c r="C111" t="s">
+        <v>137</v>
+      </c>
+      <c r="D111" t="s">
+        <v>244</v>
       </c>
       <c r="E111" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>389</v>
+        <v>291</v>
+      </c>
+      <c r="J111" t="s">
+        <v>17</v>
+      </c>
+      <c r="L111" t="s">
+        <v>465</v>
       </c>
       <c r="P111" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q111" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="112" spans="1:17">
       <c r="A112" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="C112" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D112" t="s">
-        <v>239</v>
+        <v>245</v>
+      </c>
+      <c r="E112" t="s">
+        <v>283</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="H112" t="s">
-        <v>406</v>
-      </c>
-      <c r="J112" t="s">
-        <v>17</v>
+        <v>347</v>
       </c>
       <c r="L112" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P112" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q112" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="113" spans="1:17">
       <c r="A113" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B113" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C113" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D113" t="s">
-        <v>255</v>
+        <v>246</v>
+      </c>
+      <c r="E113" t="s">
+        <v>284</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="L113" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="P113" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q113" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="114" spans="1:17">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C114" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D114" t="s">
-        <v>256</v>
+        <v>247</v>
+      </c>
+      <c r="E114" t="s">
+        <v>285</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="I114" t="s">
-        <v>407</v>
-      </c>
-      <c r="J114" t="s">
-        <v>422</v>
+        <v>381</v>
       </c>
       <c r="L114" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="P114" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q114" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="115" spans="1:17">
       <c r="A115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B115" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C115" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D115" t="s">
-        <v>257</v>
+        <v>248</v>
+      </c>
+      <c r="E115" t="s">
+        <v>286</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="I115" t="s">
-        <v>407</v>
-      </c>
-      <c r="J115" t="s">
-        <v>423</v>
-      </c>
-      <c r="L115" t="s">
-        <v>493</v>
-      </c>
-      <c r="M115" t="s">
-        <v>523</v>
+        <v>382</v>
       </c>
       <c r="P115" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q115" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="1:17">
       <c r="A116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B116" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C116" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D116" t="s">
-        <v>258</v>
+        <v>249</v>
+      </c>
+      <c r="E116" t="s">
+        <v>287</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="I116" t="s">
-        <v>407</v>
-      </c>
-      <c r="J116" t="s">
-        <v>424</v>
-      </c>
-      <c r="L116" t="s">
-        <v>494</v>
-      </c>
-      <c r="M116" t="s">
-        <v>523</v>
+        <v>383</v>
+      </c>
+      <c r="H116" t="s">
+        <v>390</v>
+      </c>
+      <c r="N116" t="s">
+        <v>512</v>
       </c>
       <c r="P116" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q116" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="117" spans="1:17">
       <c r="A117" t="s">
-        <v>23</v>
-      </c>
-      <c r="B117" t="s">
-        <v>132</v>
-      </c>
-      <c r="C117" t="s">
-        <v>147</v>
-      </c>
-      <c r="D117" t="s">
-        <v>259</v>
+        <v>25</v>
+      </c>
+      <c r="E117" t="s">
+        <v>288</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="L117" t="s">
-        <v>495</v>
-      </c>
-      <c r="M117" t="s">
-        <v>524</v>
+        <v>384</v>
       </c>
       <c r="P117" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q117" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="118" spans="1:17">
       <c r="A118" t="s">
-        <v>24</v>
-      </c>
-      <c r="E118" t="s">
-        <v>297</v>
+        <v>25</v>
+      </c>
+      <c r="B118" t="s">
+        <v>130</v>
+      </c>
+      <c r="C118" t="s">
+        <v>142</v>
+      </c>
+      <c r="D118" t="s">
+        <v>250</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>395</v>
+        <v>314</v>
+      </c>
+      <c r="H118" t="s">
+        <v>390</v>
       </c>
       <c r="P118" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q118" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="119" spans="1:17">
       <c r="A119" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D119" t="s">
-        <v>260</v>
-      </c>
-      <c r="E119" t="s">
-        <v>298</v>
+        <v>251</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J119" t="s">
-        <v>17</v>
-      </c>
-      <c r="L119" t="s">
-        <v>481</v>
+        <v>385</v>
       </c>
       <c r="P119" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q119" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:17">
       <c r="A120" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C120" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D120" t="s">
-        <v>261</v>
-      </c>
-      <c r="E120" t="s">
-        <v>299</v>
+        <v>252</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="L120" t="s">
-        <v>496</v>
+        <v>386</v>
       </c>
       <c r="P120" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q120" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="121" spans="1:17">
       <c r="A121" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C121" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D121" t="s">
-        <v>262</v>
-      </c>
-      <c r="E121" t="s">
-        <v>300</v>
+        <v>253</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="L121" t="s">
-        <v>497</v>
+        <v>385</v>
       </c>
       <c r="P121" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q121" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="122" spans="1:17">
       <c r="A122" t="s">
-        <v>24</v>
-      </c>
-      <c r="B122" t="s">
-        <v>135</v>
-      </c>
-      <c r="C122" t="s">
-        <v>151</v>
-      </c>
-      <c r="D122" t="s">
-        <v>263</v>
+        <v>26</v>
       </c>
       <c r="E122" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="L122" t="s">
-        <v>498</v>
+        <v>387</v>
       </c>
       <c r="P122" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q122" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="123" spans="1:17">
       <c r="A123" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C123" t="s">
-        <v>151</v>
-      </c>
-      <c r="D123" t="s">
-        <v>264</v>
-      </c>
-      <c r="E123" t="s">
-        <v>302</v>
+        <v>134</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>398</v>
+        <v>388</v>
+      </c>
+      <c r="H123" t="s">
+        <v>390</v>
       </c>
       <c r="P123" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q123" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="124" spans="1:17">
       <c r="A124" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B124" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C124" t="s">
-        <v>156</v>
-      </c>
-      <c r="D124" t="s">
-        <v>265</v>
-      </c>
-      <c r="E124" t="s">
-        <v>303</v>
+        <v>143</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="H124" t="s">
-        <v>406</v>
-      </c>
-      <c r="N124" t="s">
-        <v>528</v>
+        <v>357</v>
       </c>
       <c r="P124" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="Q124" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17">
-      <c r="A125" t="s">
-        <v>25</v>
-      </c>
-      <c r="E125" t="s">
-        <v>304</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="P125" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q125" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="126" spans="1:17">
-      <c r="A126" t="s">
-        <v>25</v>
-      </c>
-      <c r="B126" t="s">
-        <v>138</v>
-      </c>
-      <c r="C126" t="s">
-        <v>150</v>
-      </c>
-      <c r="D126" t="s">
-        <v>266</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="H126" t="s">
-        <v>406</v>
-      </c>
-      <c r="P126" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q126" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="127" spans="1:17">
-      <c r="A127" t="s">
-        <v>25</v>
-      </c>
-      <c r="B127" t="s">
-        <v>139</v>
-      </c>
-      <c r="C127" t="s">
-        <v>148</v>
-      </c>
-      <c r="D127" t="s">
-        <v>267</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="P127" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q127" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17">
-      <c r="A128" t="s">
-        <v>25</v>
-      </c>
-      <c r="B128" t="s">
-        <v>140</v>
-      </c>
-      <c r="C128" t="s">
-        <v>149</v>
-      </c>
-      <c r="D128" t="s">
-        <v>268</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="P128" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q128" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17">
-      <c r="A129" t="s">
-        <v>25</v>
-      </c>
-      <c r="B129" t="s">
-        <v>141</v>
-      </c>
-      <c r="C129" t="s">
-        <v>150</v>
-      </c>
-      <c r="D129" t="s">
-        <v>269</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="P129" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q129" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17">
-      <c r="A130" t="s">
-        <v>26</v>
-      </c>
-      <c r="E130" t="s">
-        <v>305</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="P130" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q130" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="131" spans="1:17">
-      <c r="A131" t="s">
-        <v>26</v>
-      </c>
-      <c r="B131" t="s">
-        <v>142</v>
-      </c>
-      <c r="C131" t="s">
-        <v>142</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="H131" t="s">
-        <v>406</v>
-      </c>
-      <c r="P131" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q131" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17">
-      <c r="A132" t="s">
-        <v>26</v>
-      </c>
-      <c r="B132" t="s">
-        <v>143</v>
-      </c>
-      <c r="C132" t="s">
-        <v>151</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="P132" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q132" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -5722,79 +5514,79 @@
     <hyperlink ref="F49" r:id="rId45"/>
     <hyperlink ref="F50" r:id="rId46"/>
     <hyperlink ref="F51" r:id="rId47"/>
-    <hyperlink ref="F56" r:id="rId48"/>
-    <hyperlink ref="F57" r:id="rId49"/>
-    <hyperlink ref="F62" r:id="rId50"/>
-    <hyperlink ref="F63" r:id="rId51"/>
-    <hyperlink ref="F64" r:id="rId52"/>
-    <hyperlink ref="F65" r:id="rId53"/>
-    <hyperlink ref="F66" r:id="rId54"/>
-    <hyperlink ref="F67" r:id="rId55"/>
-    <hyperlink ref="F68" r:id="rId56"/>
-    <hyperlink ref="F69" r:id="rId57"/>
-    <hyperlink ref="F70" r:id="rId58"/>
-    <hyperlink ref="F71" r:id="rId59"/>
-    <hyperlink ref="F72" r:id="rId60"/>
-    <hyperlink ref="F73" r:id="rId61"/>
-    <hyperlink ref="F74" r:id="rId62"/>
-    <hyperlink ref="F75" r:id="rId63"/>
-    <hyperlink ref="F76" r:id="rId64"/>
-    <hyperlink ref="F77" r:id="rId65"/>
-    <hyperlink ref="F78" r:id="rId66"/>
-    <hyperlink ref="F79" r:id="rId67"/>
-    <hyperlink ref="F80" r:id="rId68"/>
-    <hyperlink ref="F81" r:id="rId69"/>
-    <hyperlink ref="F82" r:id="rId70"/>
-    <hyperlink ref="F83" r:id="rId71"/>
-    <hyperlink ref="F84" r:id="rId72"/>
-    <hyperlink ref="F85" r:id="rId73"/>
-    <hyperlink ref="F86" r:id="rId74"/>
-    <hyperlink ref="F87" r:id="rId75"/>
-    <hyperlink ref="F88" r:id="rId76"/>
-    <hyperlink ref="F89" r:id="rId77"/>
-    <hyperlink ref="F90" r:id="rId78"/>
-    <hyperlink ref="F91" r:id="rId79"/>
-    <hyperlink ref="F92" r:id="rId80"/>
-    <hyperlink ref="F93" r:id="rId81" location="comment"/>
-    <hyperlink ref="F94" r:id="rId82"/>
-    <hyperlink ref="F95" r:id="rId83"/>
-    <hyperlink ref="F96" r:id="rId84"/>
-    <hyperlink ref="F97" r:id="rId85"/>
-    <hyperlink ref="F98" r:id="rId86"/>
-    <hyperlink ref="F99" r:id="rId87"/>
-    <hyperlink ref="F100" r:id="rId88"/>
-    <hyperlink ref="F101" r:id="rId89"/>
-    <hyperlink ref="F102" r:id="rId90"/>
-    <hyperlink ref="F103" r:id="rId91"/>
-    <hyperlink ref="F104" r:id="rId92"/>
-    <hyperlink ref="F105" r:id="rId93"/>
-    <hyperlink ref="F106" r:id="rId94"/>
-    <hyperlink ref="F107" r:id="rId95"/>
-    <hyperlink ref="F108" r:id="rId96"/>
-    <hyperlink ref="F109" r:id="rId97"/>
-    <hyperlink ref="F110" r:id="rId98"/>
-    <hyperlink ref="F111" r:id="rId99"/>
-    <hyperlink ref="F112" r:id="rId100"/>
-    <hyperlink ref="F113" r:id="rId101"/>
-    <hyperlink ref="F114" r:id="rId102"/>
-    <hyperlink ref="F115" r:id="rId103"/>
-    <hyperlink ref="F116" r:id="rId104"/>
-    <hyperlink ref="F117" r:id="rId105"/>
-    <hyperlink ref="F118" r:id="rId106"/>
-    <hyperlink ref="F119" r:id="rId107"/>
-    <hyperlink ref="F120" r:id="rId108"/>
-    <hyperlink ref="F121" r:id="rId109"/>
-    <hyperlink ref="F122" r:id="rId110"/>
-    <hyperlink ref="F123" r:id="rId111"/>
-    <hyperlink ref="F124" r:id="rId112"/>
-    <hyperlink ref="F125" r:id="rId113"/>
-    <hyperlink ref="F126" r:id="rId114"/>
-    <hyperlink ref="F127" r:id="rId115"/>
-    <hyperlink ref="F128" r:id="rId116"/>
-    <hyperlink ref="F129" r:id="rId117"/>
-    <hyperlink ref="F130" r:id="rId118"/>
-    <hyperlink ref="F131" r:id="rId119"/>
-    <hyperlink ref="F132" r:id="rId120" location="comment"/>
+    <hyperlink ref="F52" r:id="rId48"/>
+    <hyperlink ref="F53" r:id="rId49"/>
+    <hyperlink ref="F54" r:id="rId50"/>
+    <hyperlink ref="F55" r:id="rId51"/>
+    <hyperlink ref="F56" r:id="rId52"/>
+    <hyperlink ref="F57" r:id="rId53"/>
+    <hyperlink ref="F58" r:id="rId54"/>
+    <hyperlink ref="F59" r:id="rId55"/>
+    <hyperlink ref="F60" r:id="rId56"/>
+    <hyperlink ref="F61" r:id="rId57"/>
+    <hyperlink ref="F62" r:id="rId58"/>
+    <hyperlink ref="F63" r:id="rId59"/>
+    <hyperlink ref="F64" r:id="rId60"/>
+    <hyperlink ref="F65" r:id="rId61"/>
+    <hyperlink ref="F66" r:id="rId62"/>
+    <hyperlink ref="F67" r:id="rId63"/>
+    <hyperlink ref="F68" r:id="rId64"/>
+    <hyperlink ref="F69" r:id="rId65"/>
+    <hyperlink ref="F70" r:id="rId66"/>
+    <hyperlink ref="F71" r:id="rId67"/>
+    <hyperlink ref="F72" r:id="rId68"/>
+    <hyperlink ref="F73" r:id="rId69"/>
+    <hyperlink ref="F74" r:id="rId70"/>
+    <hyperlink ref="F75" r:id="rId71"/>
+    <hyperlink ref="F76" r:id="rId72"/>
+    <hyperlink ref="F77" r:id="rId73"/>
+    <hyperlink ref="F78" r:id="rId74"/>
+    <hyperlink ref="F79" r:id="rId75"/>
+    <hyperlink ref="F80" r:id="rId76"/>
+    <hyperlink ref="F81" r:id="rId77"/>
+    <hyperlink ref="F82" r:id="rId78"/>
+    <hyperlink ref="F83" r:id="rId79"/>
+    <hyperlink ref="F84" r:id="rId80"/>
+    <hyperlink ref="F85" r:id="rId81" location="comment"/>
+    <hyperlink ref="F86" r:id="rId82"/>
+    <hyperlink ref="F87" r:id="rId83"/>
+    <hyperlink ref="F88" r:id="rId84"/>
+    <hyperlink ref="F89" r:id="rId85"/>
+    <hyperlink ref="F90" r:id="rId86"/>
+    <hyperlink ref="F91" r:id="rId87"/>
+    <hyperlink ref="F92" r:id="rId88"/>
+    <hyperlink ref="F93" r:id="rId89"/>
+    <hyperlink ref="F94" r:id="rId90"/>
+    <hyperlink ref="F95" r:id="rId91"/>
+    <hyperlink ref="F96" r:id="rId92"/>
+    <hyperlink ref="F97" r:id="rId93"/>
+    <hyperlink ref="F98" r:id="rId94"/>
+    <hyperlink ref="F99" r:id="rId95"/>
+    <hyperlink ref="F100" r:id="rId96"/>
+    <hyperlink ref="F101" r:id="rId97"/>
+    <hyperlink ref="F102" r:id="rId98"/>
+    <hyperlink ref="F103" r:id="rId99"/>
+    <hyperlink ref="F104" r:id="rId100"/>
+    <hyperlink ref="F105" r:id="rId101"/>
+    <hyperlink ref="F106" r:id="rId102"/>
+    <hyperlink ref="F107" r:id="rId103"/>
+    <hyperlink ref="F108" r:id="rId104"/>
+    <hyperlink ref="F109" r:id="rId105"/>
+    <hyperlink ref="F110" r:id="rId106"/>
+    <hyperlink ref="F111" r:id="rId107"/>
+    <hyperlink ref="F112" r:id="rId108"/>
+    <hyperlink ref="F113" r:id="rId109"/>
+    <hyperlink ref="F114" r:id="rId110"/>
+    <hyperlink ref="F115" r:id="rId111"/>
+    <hyperlink ref="F116" r:id="rId112"/>
+    <hyperlink ref="F117" r:id="rId113"/>
+    <hyperlink ref="F118" r:id="rId114"/>
+    <hyperlink ref="F119" r:id="rId115"/>
+    <hyperlink ref="F120" r:id="rId116"/>
+    <hyperlink ref="F121" r:id="rId117"/>
+    <hyperlink ref="F122" r:id="rId118"/>
+    <hyperlink ref="F123" r:id="rId119"/>
+    <hyperlink ref="F124" r:id="rId120" location="comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore (data model): fix expressions for shipment registration
</commit_message>
<xml_diff>
--- a/files/imdhub-site.xlsx
+++ b/files/imdhub-site.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="519">
   <si>
     <t>tableName</t>
   </si>
@@ -247,6 +247,9 @@
     <t>clinical metadata completeness</t>
   </si>
   <si>
+    <t>biospeciment information</t>
+  </si>
+  <si>
     <t>biospecimen id</t>
   </si>
   <si>
@@ -281,6 +284,9 @@
   </si>
   <si>
     <t>reason not collected</t>
+  </si>
+  <si>
+    <t>shipment information</t>
   </si>
   <si>
     <t>shipment registration</t>
@@ -849,6 +855,12 @@
   </si>
   <si>
     <t>provide examples; different plastic ware, sample mix up, sample lost, etc.</t>
+  </si>
+  <si>
+    <t>When the specimen is selected for shipment. You will be able to see the shipment information below and be able to indicate if a specimen was received.</t>
+  </si>
+  <si>
+    <t>If the specimen was shipped, the shipment information will be displayed here.</t>
   </si>
   <si>
     <t>Mangement of the shipment of biospecimens</t>
@@ -1409,11 +1421,8 @@
     <t>if (!wasCollected &amp;&amp; (reasonNotCollected === null || reasonNotCollected === "")) "Please provide a reason why the sample was not collected"</t>
   </si>
   <si>
-    <t>if (shipmentRegistration !== null &amp;&amp; specimenReceived === null ) "Indicate if the specimen was received at the destination point"</t>
-  </si>
-  <si>
     <t>(function() {
-  if (shipmentRegistration !== null &amp;&amp; specimenReceived !== null) {
+  if (specimenReceived !== null) {
     if (!specimenReceived &amp;&amp; reasonNotReceived === null) {
       return "Please provide a reason the specimen was not received"
     } 
@@ -1422,7 +1431,7 @@
   </si>
   <si>
     <t>(function() {
-  if (shipmentRegistration !== null &amp;&amp; specimenReceived !== null) {
+  if (specimenReceived !== null) {
     if (!specimenReceived &amp;&amp; reasonNotReceived !== null) {
        if (reasonNotReceived.name === "Other") {
         return "Please provide a reason if there was another issue with the shipment";
@@ -1570,6 +1579,9 @@
     <t>participantIsVerified !== null</t>
   </si>
   <si>
+    <t>FALSE</t>
+  </si>
+  <si>
     <t>specimenType !== null ? (["PAXgene-RNA", "EDTA-Blood/DNA"].includes(specimenType.name)) : false</t>
   </si>
   <si>
@@ -1591,22 +1603,10 @@
     <t>wasCollected === false</t>
   </si>
   <si>
-    <t>shipmentRegistration !== null</t>
-  </si>
-  <si>
-    <t>shipmentRegistration !== null &amp;&amp; specimenReceived === false</t>
-  </si>
-  <si>
-    <t>(function() {
-  if (shipmentRegistration !== null &amp;&amp; specimenReceived !== null) {
-    if (!specimenReceived &amp;&amp; reasonNotReceived !== null) {
-      if (reasonNotReceived.name === "Other") {
-        return true;
-      }
-    }
-  }
-  return false;
-})();</t>
+    <t>specimenReceived !== null ? specimenReceived === false : false</t>
+  </si>
+  <si>
+    <t>reasonNotReceived !== null ? reasonNotReceived.name === "Other" : false</t>
   </si>
   <si>
     <t>participant !== null</t>
@@ -1681,9 +1681,6 @@
     }
   }
 })();</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -2028,7 +2025,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q124"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2092,16 +2089,16 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="P2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2112,13 +2109,13 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="P3" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q3" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2129,31 +2126,31 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="H4" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="J4" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="L4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="P4" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q4" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2164,28 +2161,28 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="I5" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J5" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="L5" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="P5" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q5" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2196,25 +2193,25 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="L6" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="P6" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q6" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2225,25 +2222,25 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="L7" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="O7" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="P7" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q7" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2254,28 +2251,28 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="I8" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J8" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="L8" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="P8" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q8" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2286,28 +2283,28 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I9" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J9" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="L9" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="P9" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q9" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2318,19 +2315,19 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="P10" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q10" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2341,31 +2338,31 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="I11" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J11" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="L11" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="P11" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q11" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2376,19 +2373,19 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="P12" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q12" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2399,25 +2396,25 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="L13" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="P13" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q13" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2428,22 +2425,22 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="L14" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="P14" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q14" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2454,22 +2451,22 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="L15" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="P15" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q15" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2480,22 +2477,22 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="L16" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="P16" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q16" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2506,22 +2503,22 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D17" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="L17" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="P17" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q17" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2532,22 +2529,22 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="L18" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="P18" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q18" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2558,31 +2555,31 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="I19" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J19" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="L19" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="M19" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="P19" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q19" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2593,22 +2590,22 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="L20" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="P20" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q20" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2619,28 +2616,28 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E21" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="L21" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="M21" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="P21" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q21" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2651,28 +2648,28 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E22" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="L22" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="M22" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="P22" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q22" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2683,25 +2680,25 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="L23" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="M23" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="P23" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q23" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2712,25 +2709,25 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="L24" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="M24" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="P24" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q24" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2741,25 +2738,25 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D25" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="L25" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="M25" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="P25" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q25" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2770,16 +2767,16 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="P26" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q26" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2790,25 +2787,25 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E27" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="L27" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="P27" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q27" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2819,34 +2816,34 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E28" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="I28" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J28" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="L28" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="M28" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="P28" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q28" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2857,25 +2854,25 @@
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="L29" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="M29" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="P29" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q29" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2886,16 +2883,16 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="P30" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q30" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2906,28 +2903,28 @@
         <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E31" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="L31" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="M31" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P31" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q31" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2938,25 +2935,25 @@
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="L32" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="M32" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P32" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q32" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2967,25 +2964,25 @@
         <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="L33" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="M33" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P33" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q33" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2996,28 +2993,28 @@
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E34" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="L34" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="M34" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P34" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q34" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -3028,28 +3025,28 @@
         <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E35" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="L35" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="M35" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P35" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q35" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -3060,28 +3057,28 @@
         <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E36" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="L36" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="M36" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="P36" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q36" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -3092,22 +3089,22 @@
         <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L37" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="P37" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q37" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3118,25 +3115,25 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D38" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="L38" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="M38" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="P38" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q38" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -3147,19 +3144,19 @@
         <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D39" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="P39" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q39" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -3170,25 +3167,25 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E40" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="G40" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="M40" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="P40" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q40" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3199,22 +3196,22 @@
         <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E41" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="M41" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="P41" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q41" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -3222,16 +3219,16 @@
         <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="P42" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q42" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3242,31 +3239,34 @@
         <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D43" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E43" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="H43" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="L43" t="s">
-        <v>440</v>
+        <v>444</v>
+      </c>
+      <c r="M43" t="s">
+        <v>495</v>
       </c>
       <c r="N43" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="P43" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q43" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3277,28 +3277,28 @@
         <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D44" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E44" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="J44" t="s">
         <v>17</v>
       </c>
       <c r="L44" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="P44" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q44" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3309,22 +3309,22 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="L45" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="P45" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q45" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -3335,31 +3335,31 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D46" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E46" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="I46" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J46" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="L46" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="P46" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q46" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -3370,25 +3370,25 @@
         <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D47" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E47" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="L47" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="P47" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q47" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -3399,22 +3399,22 @@
         <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D48" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="L48" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="P48" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q48" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -3425,16 +3425,16 @@
         <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="P49" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q49" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3445,22 +3445,22 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="J50" t="s">
         <v>19</v>
       </c>
       <c r="K50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P50" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q50" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -3471,22 +3471,22 @@
         <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E51" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="P51" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q51" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -3497,19 +3497,19 @@
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="P52" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q52" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -3520,19 +3520,19 @@
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="P53" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q53" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="54" spans="1:17">
@@ -3540,16 +3540,16 @@
         <v>19</v>
       </c>
       <c r="E54" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="P54" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q54" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -3560,25 +3560,16 @@
         <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>142</v>
-      </c>
-      <c r="D55" t="s">
-        <v>194</v>
+        <v>147</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="H55" t="s">
-        <v>390</v>
-      </c>
-      <c r="L55" t="s">
-        <v>446</v>
+        <v>294</v>
       </c>
       <c r="P55" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q55" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -3589,31 +3580,25 @@
         <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D56" t="s">
-        <v>195</v>
-      </c>
-      <c r="E56" t="s">
-        <v>276</v>
+        <v>196</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="I56" t="s">
-        <v>391</v>
-      </c>
-      <c r="J56" t="s">
-        <v>400</v>
+        <v>294</v>
+      </c>
+      <c r="H56" t="s">
+        <v>394</v>
       </c>
       <c r="L56" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="P56" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q56" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -3624,28 +3609,31 @@
         <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="E57" t="s">
+        <v>278</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="M57" t="s">
-        <v>492</v>
-      </c>
-      <c r="N57" t="s">
-        <v>510</v>
-      </c>
-      <c r="O57" t="s">
-        <v>514</v>
+        <v>338</v>
+      </c>
+      <c r="I57" t="s">
+        <v>395</v>
+      </c>
+      <c r="J57" t="s">
+        <v>404</v>
+      </c>
+      <c r="L57" t="s">
+        <v>451</v>
       </c>
       <c r="P57" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q57" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -3656,28 +3644,28 @@
         <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="L58" t="s">
-        <v>448</v>
+        <v>339</v>
       </c>
       <c r="M58" t="s">
-        <v>493</v>
+        <v>496</v>
+      </c>
+      <c r="N58" t="s">
+        <v>513</v>
       </c>
       <c r="O58" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="P58" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q58" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -3688,25 +3676,28 @@
         <v>81</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="J59" t="s">
-        <v>18</v>
+        <v>340</v>
       </c>
       <c r="L59" t="s">
-        <v>449</v>
+        <v>452</v>
+      </c>
+      <c r="M59" t="s">
+        <v>497</v>
+      </c>
+      <c r="O59" t="s">
+        <v>518</v>
       </c>
       <c r="P59" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q59" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -3717,22 +3708,25 @@
         <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D60" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
+      </c>
+      <c r="J60" t="s">
+        <v>18</v>
       </c>
       <c r="L60" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="P60" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q60" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -3743,25 +3737,22 @@
         <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D61" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="L61" t="s">
-        <v>451</v>
-      </c>
-      <c r="M61" t="s">
-        <v>494</v>
+        <v>454</v>
       </c>
       <c r="P61" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q61" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -3775,22 +3766,22 @@
         <v>143</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="L62" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="M62" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="P62" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q62" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -3801,31 +3792,25 @@
         <v>85</v>
       </c>
       <c r="C63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I63" t="s">
-        <v>391</v>
-      </c>
-      <c r="J63" t="s">
-        <v>401</v>
+        <v>344</v>
       </c>
       <c r="L63" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="M63" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="P63" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q63" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -3836,28 +3821,31 @@
         <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
-      </c>
-      <c r="E64" t="s">
-        <v>277</v>
+        <v>204</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>339</v>
+        <v>345</v>
+      </c>
+      <c r="I64" t="s">
+        <v>395</v>
+      </c>
+      <c r="J64" t="s">
+        <v>405</v>
       </c>
       <c r="L64" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="M64" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="P64" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q64" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -3871,22 +3859,25 @@
         <v>143</v>
       </c>
       <c r="D65" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="E65" t="s">
+        <v>279</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="L65" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="M65" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="P65" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q65" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="66" spans="1:17">
@@ -3897,25 +3888,25 @@
         <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D66" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="L66" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="M66" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="P66" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q66" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -3926,22 +3917,25 @@
         <v>89</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="D67" t="s">
+        <v>207</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="J67" t="s">
-        <v>20</v>
-      </c>
-      <c r="K67" t="s">
-        <v>95</v>
+        <v>346</v>
+      </c>
+      <c r="L67" t="s">
+        <v>460</v>
+      </c>
+      <c r="M67" t="s">
+        <v>502</v>
       </c>
       <c r="P67" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q67" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -3952,25 +3946,19 @@
         <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
-      </c>
-      <c r="D68" t="s">
-        <v>206</v>
+        <v>147</v>
+      </c>
+      <c r="E68" t="s">
+        <v>280</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="L68" t="s">
-        <v>457</v>
-      </c>
-      <c r="M68" t="s">
-        <v>499</v>
+        <v>347</v>
       </c>
       <c r="P68" t="s">
-        <v>516</v>
+        <v>393</v>
       </c>
       <c r="Q68" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -3981,31 +3969,25 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
-      </c>
-      <c r="D69" t="s">
-        <v>207</v>
+        <v>146</v>
+      </c>
+      <c r="E69" t="s">
+        <v>281</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="I69" t="s">
-        <v>391</v>
+        <v>347</v>
       </c>
       <c r="J69" t="s">
-        <v>402</v>
-      </c>
-      <c r="L69" t="s">
-        <v>458</v>
-      </c>
-      <c r="M69" t="s">
-        <v>500</v>
+        <v>20</v>
+      </c>
+      <c r="K69" t="s">
+        <v>97</v>
       </c>
       <c r="P69" t="s">
-        <v>516</v>
+        <v>393</v>
       </c>
       <c r="Q69" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -4022,91 +4004,94 @@
         <v>208</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="L70" t="s">
-        <v>459</v>
-      </c>
-      <c r="M70" t="s">
-        <v>501</v>
+        <v>348</v>
       </c>
       <c r="P70" t="s">
-        <v>516</v>
+        <v>393</v>
       </c>
       <c r="Q70" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="71" spans="1:17">
       <c r="A71" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71" t="s">
-        <v>278</v>
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" t="s">
+        <v>140</v>
+      </c>
+      <c r="D71" t="s">
+        <v>209</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>343</v>
+        <v>349</v>
+      </c>
+      <c r="I71" t="s">
+        <v>395</v>
+      </c>
+      <c r="J71" t="s">
+        <v>406</v>
+      </c>
+      <c r="L71" t="s">
+        <v>461</v>
+      </c>
+      <c r="M71" t="s">
+        <v>503</v>
       </c>
       <c r="P71" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q71" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D72" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="H72" t="s">
-        <v>390</v>
-      </c>
-      <c r="N72" t="s">
-        <v>511</v>
+        <v>349</v>
+      </c>
+      <c r="L72" t="s">
+        <v>462</v>
+      </c>
+      <c r="M72" t="s">
+        <v>504</v>
       </c>
       <c r="P72" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q72" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>20</v>
       </c>
-      <c r="B73" t="s">
-        <v>94</v>
-      </c>
-      <c r="C73" t="s">
-        <v>139</v>
-      </c>
-      <c r="D73" t="s">
-        <v>210</v>
+      <c r="E73" t="s">
+        <v>282</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="L73" t="s">
-        <v>460</v>
-      </c>
       <c r="P73" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q73" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -4117,25 +4102,25 @@
         <v>95</v>
       </c>
       <c r="C74" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D74" t="s">
         <v>211</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="J74" t="s">
-        <v>19</v>
-      </c>
-      <c r="L74" t="s">
-        <v>461</v>
+        <v>350</v>
+      </c>
+      <c r="H74" t="s">
+        <v>394</v>
+      </c>
+      <c r="N74" t="s">
+        <v>514</v>
       </c>
       <c r="P74" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q74" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -4146,28 +4131,22 @@
         <v>96</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D75" t="s">
         <v>212</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="I75" t="s">
-        <v>391</v>
-      </c>
-      <c r="J75" t="s">
-        <v>402</v>
+        <v>351</v>
       </c>
       <c r="L75" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="P75" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q75" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -4178,19 +4157,25 @@
         <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D76" t="s">
         <v>213</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>349</v>
+        <v>294</v>
+      </c>
+      <c r="J76" t="s">
+        <v>19</v>
+      </c>
+      <c r="L76" t="s">
+        <v>464</v>
       </c>
       <c r="P76" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q76" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -4201,19 +4186,28 @@
         <v>98</v>
       </c>
       <c r="C77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D77" t="s">
         <v>214</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
+      </c>
+      <c r="I77" t="s">
+        <v>395</v>
+      </c>
+      <c r="J77" t="s">
+        <v>406</v>
+      </c>
+      <c r="L77" t="s">
+        <v>465</v>
       </c>
       <c r="P77" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q77" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -4224,19 +4218,19 @@
         <v>99</v>
       </c>
       <c r="C78" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D78" t="s">
         <v>215</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="P78" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q78" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -4247,19 +4241,19 @@
         <v>100</v>
       </c>
       <c r="C79" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D79" t="s">
         <v>216</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="P79" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q79" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4270,19 +4264,19 @@
         <v>101</v>
       </c>
       <c r="C80" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="D80" t="s">
         <v>217</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="P80" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q80" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="81" spans="1:17">
@@ -4293,28 +4287,19 @@
         <v>102</v>
       </c>
       <c r="C81" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D81" t="s">
         <v>218</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="I81" t="s">
-        <v>391</v>
-      </c>
-      <c r="J81" t="s">
-        <v>393</v>
-      </c>
-      <c r="L81" t="s">
-        <v>463</v>
+        <v>355</v>
       </c>
       <c r="P81" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q81" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="82" spans="1:17">
@@ -4325,28 +4310,19 @@
         <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
         <v>219</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="I82" t="s">
-        <v>391</v>
-      </c>
-      <c r="J82" t="s">
-        <v>393</v>
-      </c>
-      <c r="L82" t="s">
-        <v>464</v>
+        <v>356</v>
       </c>
       <c r="P82" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q82" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -4357,19 +4333,28 @@
         <v>104</v>
       </c>
       <c r="C83" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D83" t="s">
         <v>220</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
+      </c>
+      <c r="I83" t="s">
+        <v>395</v>
+      </c>
+      <c r="J83" t="s">
+        <v>397</v>
+      </c>
+      <c r="L83" t="s">
+        <v>466</v>
       </c>
       <c r="P83" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q83" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -4380,19 +4365,28 @@
         <v>105</v>
       </c>
       <c r="C84" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D84" t="s">
         <v>221</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
+      </c>
+      <c r="I84" t="s">
+        <v>395</v>
+      </c>
+      <c r="J84" t="s">
+        <v>397</v>
+      </c>
+      <c r="L84" t="s">
+        <v>467</v>
       </c>
       <c r="P84" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q84" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -4400,100 +4394,85 @@
         <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D85" t="s">
         <v>222</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="P85" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q85" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="86" spans="1:17">
       <c r="A86" t="s">
-        <v>21</v>
-      </c>
-      <c r="E86" t="s">
-        <v>279</v>
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" t="s">
+        <v>144</v>
+      </c>
+      <c r="D86" t="s">
+        <v>223</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="P86" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q86" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="87" spans="1:17">
       <c r="A87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C87" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D87" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="H87" t="s">
-        <v>390</v>
-      </c>
-      <c r="J87" t="s">
-        <v>17</v>
-      </c>
-      <c r="L87" t="s">
-        <v>465</v>
+        <v>361</v>
       </c>
       <c r="P87" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q87" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="88" spans="1:17">
       <c r="A88" t="s">
         <v>21</v>
       </c>
-      <c r="B88" t="s">
-        <v>106</v>
-      </c>
-      <c r="C88" t="s">
-        <v>141</v>
-      </c>
-      <c r="D88" t="s">
-        <v>224</v>
+      <c r="E88" t="s">
+        <v>283</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="L88" t="s">
-        <v>466</v>
-      </c>
-      <c r="M88" t="s">
-        <v>502</v>
+        <v>362</v>
       </c>
       <c r="P88" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q88" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="89" spans="1:17">
@@ -4501,34 +4480,31 @@
         <v>21</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="C89" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D89" t="s">
         <v>225</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="I89" t="s">
-        <v>391</v>
+        <v>295</v>
+      </c>
+      <c r="H89" t="s">
+        <v>394</v>
       </c>
       <c r="J89" t="s">
-        <v>403</v>
+        <v>17</v>
       </c>
       <c r="L89" t="s">
-        <v>467</v>
-      </c>
-      <c r="M89" t="s">
-        <v>503</v>
+        <v>468</v>
       </c>
       <c r="P89" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q89" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="90" spans="1:17">
@@ -4539,25 +4515,25 @@
         <v>108</v>
       </c>
       <c r="C90" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D90" t="s">
         <v>226</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="L90" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="M90" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="P90" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q90" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -4568,31 +4544,31 @@
         <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D91" t="s">
         <v>227</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="I91" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J91" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="L91" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M91" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="P91" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q91" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="92" spans="1:17">
@@ -4603,25 +4579,25 @@
         <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D92" t="s">
         <v>228</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="L92" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="M92" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="P92" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q92" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="93" spans="1:17">
@@ -4632,31 +4608,31 @@
         <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D93" t="s">
         <v>229</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="I93" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J93" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="L93" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="M93" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="P93" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q93" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="94" spans="1:17">
@@ -4667,25 +4643,25 @@
         <v>112</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D94" t="s">
         <v>230</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="L94" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="M94" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P94" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q94" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="95" spans="1:17">
@@ -4696,25 +4672,31 @@
         <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D95" t="s">
         <v>231</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
+      </c>
+      <c r="I95" t="s">
+        <v>395</v>
+      </c>
+      <c r="J95" t="s">
+        <v>409</v>
       </c>
       <c r="L95" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="M95" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P95" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q95" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="96" spans="1:17">
@@ -4725,80 +4707,83 @@
         <v>114</v>
       </c>
       <c r="C96" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D96" t="s">
         <v>232</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="L96" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M96" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="P96" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q96" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="97" spans="1:17">
       <c r="A97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B97" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="C97" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D97" t="s">
         <v>233</v>
       </c>
-      <c r="E97" t="s">
-        <v>271</v>
-      </c>
       <c r="F97" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="H97" t="s">
-        <v>390</v>
-      </c>
-      <c r="J97" t="s">
-        <v>17</v>
+        <v>370</v>
+      </c>
+      <c r="L97" t="s">
+        <v>476</v>
+      </c>
+      <c r="M97" t="s">
+        <v>508</v>
       </c>
       <c r="P97" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q97" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="98" spans="1:17">
       <c r="A98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C98" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D98" t="s">
         <v>234</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
+      </c>
+      <c r="L98" t="s">
+        <v>477</v>
+      </c>
+      <c r="M98" t="s">
+        <v>509</v>
       </c>
       <c r="P98" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q98" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="1:17">
@@ -4806,22 +4791,31 @@
         <v>22</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="C99" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D99" t="s">
         <v>235</v>
       </c>
+      <c r="E99" t="s">
+        <v>273</v>
+      </c>
       <c r="F99" s="1" t="s">
-        <v>369</v>
+        <v>295</v>
+      </c>
+      <c r="H99" t="s">
+        <v>394</v>
+      </c>
+      <c r="J99" t="s">
+        <v>17</v>
       </c>
       <c r="P99" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q99" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100" spans="1:17">
@@ -4832,19 +4826,19 @@
         <v>117</v>
       </c>
       <c r="C100" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D100" t="s">
         <v>236</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="P100" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q100" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="101" spans="1:17">
@@ -4855,19 +4849,19 @@
         <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D101" t="s">
         <v>237</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="P101" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q101" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="102" spans="1:17">
@@ -4878,94 +4872,82 @@
         <v>119</v>
       </c>
       <c r="C102" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D102" t="s">
         <v>238</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="P102" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q102" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="103" spans="1:17">
       <c r="A103" t="s">
-        <v>23</v>
-      </c>
-      <c r="E103" t="s">
-        <v>280</v>
+        <v>22</v>
+      </c>
+      <c r="B103" t="s">
+        <v>120</v>
+      </c>
+      <c r="C103" t="s">
+        <v>144</v>
+      </c>
+      <c r="D103" t="s">
+        <v>239</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="P103" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q103" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="104" spans="1:17">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B104" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="C104" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D104" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="H104" t="s">
-        <v>390</v>
-      </c>
-      <c r="J104" t="s">
-        <v>17</v>
-      </c>
-      <c r="L104" t="s">
-        <v>465</v>
+        <v>376</v>
       </c>
       <c r="P104" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q104" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="105" spans="1:17">
       <c r="A105" t="s">
         <v>23</v>
       </c>
-      <c r="B105" t="s">
-        <v>120</v>
-      </c>
-      <c r="C105" t="s">
-        <v>139</v>
-      </c>
-      <c r="D105" t="s">
-        <v>239</v>
+      <c r="E105" t="s">
+        <v>284</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="L105" t="s">
-        <v>475</v>
+        <v>377</v>
       </c>
       <c r="P105" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q105" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="106" spans="1:17">
@@ -4973,31 +4955,31 @@
         <v>23</v>
       </c>
       <c r="B106" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="C106" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D106" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="I106" t="s">
-        <v>391</v>
+        <v>295</v>
+      </c>
+      <c r="H106" t="s">
+        <v>394</v>
       </c>
       <c r="J106" t="s">
-        <v>406</v>
+        <v>17</v>
       </c>
       <c r="L106" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="P106" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q106" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="107" spans="1:17">
@@ -5008,31 +4990,22 @@
         <v>122</v>
       </c>
       <c r="C107" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D107" t="s">
         <v>241</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="I107" t="s">
-        <v>391</v>
-      </c>
-      <c r="J107" t="s">
-        <v>407</v>
+        <v>378</v>
       </c>
       <c r="L107" t="s">
-        <v>477</v>
-      </c>
-      <c r="M107" t="s">
-        <v>507</v>
+        <v>478</v>
       </c>
       <c r="P107" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q107" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="108" spans="1:17">
@@ -5043,31 +5016,28 @@
         <v>123</v>
       </c>
       <c r="C108" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D108" t="s">
         <v>242</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="I108" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="J108" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="L108" t="s">
-        <v>478</v>
-      </c>
-      <c r="M108" t="s">
-        <v>507</v>
+        <v>479</v>
       </c>
       <c r="P108" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q108" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="109" spans="1:17">
@@ -5078,103 +5048,112 @@
         <v>124</v>
       </c>
       <c r="C109" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D109" t="s">
         <v>243</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
+      </c>
+      <c r="I109" t="s">
+        <v>395</v>
+      </c>
+      <c r="J109" t="s">
+        <v>411</v>
       </c>
       <c r="L109" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M109" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="P109" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q109" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="1:17">
       <c r="A110" t="s">
-        <v>24</v>
-      </c>
-      <c r="E110" t="s">
-        <v>281</v>
+        <v>23</v>
+      </c>
+      <c r="B110" t="s">
+        <v>125</v>
+      </c>
+      <c r="C110" t="s">
+        <v>140</v>
+      </c>
+      <c r="D110" t="s">
+        <v>244</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
+      </c>
+      <c r="I110" t="s">
+        <v>395</v>
+      </c>
+      <c r="J110" t="s">
+        <v>412</v>
+      </c>
+      <c r="L110" t="s">
+        <v>481</v>
+      </c>
+      <c r="M110" t="s">
+        <v>510</v>
       </c>
       <c r="P110" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q110" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" spans="1:17">
       <c r="A111" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B111" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="C111" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D111" t="s">
-        <v>244</v>
-      </c>
-      <c r="E111" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="J111" t="s">
-        <v>17</v>
+        <v>382</v>
       </c>
       <c r="L111" t="s">
-        <v>465</v>
+        <v>482</v>
+      </c>
+      <c r="M111" t="s">
+        <v>511</v>
       </c>
       <c r="P111" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q111" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="112" spans="1:17">
       <c r="A112" t="s">
         <v>24</v>
       </c>
-      <c r="B112" t="s">
-        <v>125</v>
-      </c>
-      <c r="C112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D112" t="s">
-        <v>245</v>
-      </c>
       <c r="E112" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="L112" t="s">
-        <v>480</v>
+        <v>383</v>
       </c>
       <c r="P112" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q112" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="113" spans="1:17">
@@ -5182,28 +5161,31 @@
         <v>24</v>
       </c>
       <c r="B113" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="C113" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D113" t="s">
         <v>246</v>
       </c>
       <c r="E113" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>380</v>
+        <v>295</v>
+      </c>
+      <c r="J113" t="s">
+        <v>17</v>
       </c>
       <c r="L113" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="P113" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q113" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="114" spans="1:17">
@@ -5214,25 +5196,25 @@
         <v>127</v>
       </c>
       <c r="C114" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D114" t="s">
         <v>247</v>
       </c>
       <c r="E114" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
       <c r="L114" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="P114" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q114" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="115" spans="1:17">
@@ -5243,22 +5225,25 @@
         <v>128</v>
       </c>
       <c r="C115" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D115" t="s">
         <v>248</v>
       </c>
       <c r="E115" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
+      </c>
+      <c r="L115" t="s">
+        <v>484</v>
       </c>
       <c r="P115" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q115" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -5269,94 +5254,100 @@
         <v>129</v>
       </c>
       <c r="C116" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D116" t="s">
         <v>249</v>
       </c>
       <c r="E116" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="H116" t="s">
-        <v>390</v>
-      </c>
-      <c r="N116" t="s">
-        <v>512</v>
+        <v>385</v>
+      </c>
+      <c r="L116" t="s">
+        <v>485</v>
       </c>
       <c r="P116" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q116" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="117" spans="1:17">
       <c r="A117" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B117" t="s">
+        <v>130</v>
+      </c>
+      <c r="C117" t="s">
+        <v>145</v>
+      </c>
+      <c r="D117" t="s">
+        <v>250</v>
       </c>
       <c r="E117" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="P117" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q117" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="118" spans="1:17">
       <c r="A118" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B118" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C118" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D118" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="E118" t="s">
+        <v>291</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>314</v>
+        <v>387</v>
       </c>
       <c r="H118" t="s">
-        <v>390</v>
+        <v>394</v>
+      </c>
+      <c r="N118" t="s">
+        <v>515</v>
       </c>
       <c r="P118" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q118" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119" spans="1:17">
       <c r="A119" t="s">
         <v>25</v>
       </c>
-      <c r="B119" t="s">
-        <v>131</v>
-      </c>
-      <c r="C119" t="s">
-        <v>140</v>
-      </c>
-      <c r="D119" t="s">
-        <v>251</v>
+      <c r="E119" t="s">
+        <v>292</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="P119" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q119" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:17">
@@ -5367,19 +5358,22 @@
         <v>132</v>
       </c>
       <c r="C120" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D120" t="s">
         <v>252</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>386</v>
+        <v>318</v>
+      </c>
+      <c r="H120" t="s">
+        <v>394</v>
       </c>
       <c r="P120" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q120" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="121" spans="1:17">
@@ -5396,73 +5390,119 @@
         <v>253</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="P121" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q121" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="122" spans="1:17">
       <c r="A122" t="s">
-        <v>26</v>
-      </c>
-      <c r="E122" t="s">
-        <v>289</v>
+        <v>25</v>
+      </c>
+      <c r="B122" t="s">
+        <v>134</v>
+      </c>
+      <c r="C122" t="s">
+        <v>143</v>
+      </c>
+      <c r="D122" t="s">
+        <v>254</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="P122" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q122" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="123" spans="1:17">
       <c r="A123" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B123" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C123" t="s">
-        <v>134</v>
+        <v>144</v>
+      </c>
+      <c r="D123" t="s">
+        <v>255</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="H123" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="P123" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q123" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="124" spans="1:17">
       <c r="A124" t="s">
         <v>26</v>
       </c>
-      <c r="B124" t="s">
-        <v>135</v>
-      </c>
-      <c r="C124" t="s">
-        <v>143</v>
+      <c r="E124" t="s">
+        <v>293</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>357</v>
+        <v>391</v>
       </c>
       <c r="P124" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="Q124" t="s">
-        <v>389</v>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="A125" t="s">
+        <v>26</v>
+      </c>
+      <c r="B125" t="s">
+        <v>136</v>
+      </c>
+      <c r="C125" t="s">
+        <v>136</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H125" t="s">
+        <v>394</v>
+      </c>
+      <c r="P125" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
+      <c r="A126" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" t="s">
+        <v>137</v>
+      </c>
+      <c r="C126" t="s">
+        <v>145</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="P126" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -5547,9 +5587,9 @@
     <hyperlink ref="F82" r:id="rId78"/>
     <hyperlink ref="F83" r:id="rId79"/>
     <hyperlink ref="F84" r:id="rId80"/>
-    <hyperlink ref="F85" r:id="rId81" location="comment"/>
+    <hyperlink ref="F85" r:id="rId81"/>
     <hyperlink ref="F86" r:id="rId82"/>
-    <hyperlink ref="F87" r:id="rId83"/>
+    <hyperlink ref="F87" r:id="rId83" location="comment"/>
     <hyperlink ref="F88" r:id="rId84"/>
     <hyperlink ref="F89" r:id="rId85"/>
     <hyperlink ref="F90" r:id="rId86"/>
@@ -5586,7 +5626,9 @@
     <hyperlink ref="F121" r:id="rId117"/>
     <hyperlink ref="F122" r:id="rId118"/>
     <hyperlink ref="F123" r:id="rId119"/>
-    <hyperlink ref="F124" r:id="rId120" location="comment"/>
+    <hyperlink ref="F124" r:id="rId120"/>
+    <hyperlink ref="F125" r:id="rId121"/>
+    <hyperlink ref="F126" r:id="rId122" location="comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
data (fixes): revisions of data model
</commit_message>
<xml_diff>
--- a/files/imdhub-site.xlsx
+++ b/files/imdhub-site.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="527">
   <si>
     <t>tableName</t>
   </si>
@@ -124,6 +124,9 @@
     <t>cohort assignment</t>
   </si>
   <si>
+    <t>iembase diagnosis</t>
+  </si>
+  <si>
     <t>participant consent</t>
   </si>
   <si>
@@ -247,7 +250,7 @@
     <t>clinical metadata completeness</t>
   </si>
   <si>
-    <t>biospeciment information</t>
+    <t>biospecimen information</t>
   </si>
   <si>
     <t>biospecimen id</t>
@@ -494,6 +497,9 @@
   </si>
   <si>
     <t>Cohort assignment</t>
+  </si>
+  <si>
+    <t>Select IEMbase Nosology diagnosis</t>
   </si>
   <si>
     <t>Informed consent</t>
@@ -656,216 +662,219 @@
     <t>Enter the date of the shipment registration</t>
   </si>
   <si>
+    <t>Biospecimens to ship</t>
+  </si>
+  <si>
+    <t>Select the current status of the shipment</t>
+  </si>
+  <si>
+    <t>Enter the courier service</t>
+  </si>
+  <si>
+    <t>Enter the tracking number provided by the courier service</t>
+  </si>
+  <si>
+    <t>Enter the URL to the tracking page provided by the courier service</t>
+  </si>
+  <si>
+    <t>Enter the name of the person that is responsible for preparing and sending the shipment</t>
+  </si>
+  <si>
+    <t>Enter the date the shipment was sent</t>
+  </si>
+  <si>
+    <t>Select the origin point of the shipment</t>
+  </si>
+  <si>
+    <t>Select the destination point of the shipment</t>
+  </si>
+  <si>
+    <t>Enter the date the shipment was received at the destination point</t>
+  </si>
+  <si>
+    <t>Enter the name of the person that is responsible for receiving and unpacking the shipment</t>
+  </si>
+  <si>
+    <t>If applicable, enter additional information about the shipment</t>
+  </si>
+  <si>
+    <t>Select the participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there whole genome or exome sequencing data of the participant in storage? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the previously generated sequencing data of the participant stored with a third party sequence provider, another healthcare provider or the site? </t>
+  </si>
+  <si>
+    <t>What is the name of the third party sequence provider?</t>
+  </si>
+  <si>
+    <t>Select the participant's disease status resulting from previous genetic testing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When was the genetic testing of this sequencing data performed (MM/YY)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select from the list the sequencing system used? Only systems listed are accepted. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was the sequencing kit used? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the sequencing data previously generated been in the form of either FASTQs or CRAM files (in FASTA format), which encompass unmapped reads? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ftp secure transfer of sequencing data </t>
+  </si>
+  <si>
+    <t>Recon4IMD particpant identifier</t>
+  </si>
+  <si>
+    <t>Previous history of any surgery?</t>
+  </si>
+  <si>
+    <t>If yes, what surgery was performed and when did it occur?</t>
+  </si>
+  <si>
+    <t>Has the participant taken any medications or supplements in last 6 months?</t>
+  </si>
+  <si>
+    <t>Does the participant have any dietary restrictions or preferences?</t>
+  </si>
+  <si>
+    <t>What foods has the participant consumed within the last 24 hours?</t>
+  </si>
+  <si>
+    <t>When did the participant come off study?</t>
+  </si>
+  <si>
+    <t>Why is the participant coming off the study?</t>
+  </si>
+  <si>
+    <t>When a participant withdraws their consent, do they want their data used or deleted?</t>
+  </si>
+  <si>
+    <t>When a participant withdraws their consent, do they want their samples to be used, returned or destroyed?</t>
+  </si>
+  <si>
+    <t>If the patient has died, what is the date of death?</t>
+  </si>
+  <si>
+    <t>Participant identifier</t>
+  </si>
+  <si>
+    <t>Date of query</t>
+  </si>
+  <si>
+    <t>Reason for query</t>
+  </si>
+  <si>
+    <t>Sponsory query</t>
+  </si>
+  <si>
+    <t>Site response</t>
+  </si>
+  <si>
+    <t>Query identifier</t>
+  </si>
+  <si>
+    <t>IMD IEMbase</t>
+  </si>
+  <si>
+    <t>Prevalence data (number of patients) site specific (adult/pead)</t>
+  </si>
+  <si>
+    <t>Is the data correct (T/F)</t>
+  </si>
+  <si>
+    <t>If no, specify prevalence</t>
+  </si>
+  <si>
+    <t>Register new participants and manage existing registrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select the Recon4IMD participant identifier. The Recon4IMD ID entered here should match that assigned to the participant during sampling and recorded on the related Biospecimen worksheet.   </t>
+  </si>
+  <si>
+    <t>Date the participant was entered into the IMDhub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select the participant's cohort assignment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants or legal representatives give written informed consent to study participation and consent for the collection and analysis of both blood and urine samples, and where indicated, a fibroblast sample or a stool sample. </t>
+  </si>
+  <si>
+    <t>Participant is suspected to have an IMD and was advised on genetic testing.</t>
+  </si>
+  <si>
+    <t>Particpant is informed of all the risks and benefits.</t>
+  </si>
+  <si>
+    <t>Participants enrolled or registered with one of the following participant registries or cohort study (with ethical approval at site): U-IMD, GENOMIT or Solve-RD.</t>
+  </si>
+  <si>
+    <t>If the participant is part of a participant registry or cohort study, select the registry.</t>
+  </si>
+  <si>
+    <t>Participants have the potential to be or a confirmed carrier of an IMD pathogenic variant.</t>
+  </si>
+  <si>
+    <t>E.g., cardiovascular, diabetes, hypertension, respiratory, gastrointestinal, nervous, urinary, endocrine, musculoskeletal, mental disorders, and addiction</t>
+  </si>
+  <si>
+    <t>E.g., HIV, infectious hepatitis, tuberculposis, or Creutzfeldt-Jakob disease</t>
+  </si>
+  <si>
+    <t>Participant had a blood transfusion within the last month</t>
+  </si>
+  <si>
+    <t>An indication that the participant meets selection criteria</t>
+  </si>
+  <si>
+    <t>An indication that the participant is confirmed with the registry</t>
+  </si>
+  <si>
+    <t>Registration of visits by participant and date</t>
+  </si>
+  <si>
+    <t>To generate the visit ID, please select a participant and the type of visit</t>
+  </si>
+  <si>
+    <t>Enter the Recon4IMD participant identifier. This identifier is generated upon participant registration into the IMDhub.</t>
+  </si>
+  <si>
+    <t>The enrollment visit is the initial study visit of the participant and the follow-up visit is any study visit after the initial study visit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fasting is when a subject doesn't eat or drink anything other than water only. </t>
+  </si>
+  <si>
+    <t>Comprised of the following clinical data fields: Demographics, Patient status, Disease history [IMD diagnosis including primary mitochondrial disease (PMD), Metabolites at diagnosis, Genetic results], Medical history [Family IMD history, Other conditions], Clinical exam, body weight and height at time of visit, Disease signs and symptoms at time of visit [Clinical progression, Human Phenotype Ontology, Neuropsychological testing, PMD symptoms, PMD brain imaging results], Treatment at time of visit [Drug Treatment, Dietary treatment, Renal therapy, Non-pharmacologic therapies], Laboratory analysis at time of visit [ERKNet parameters, Metabolites at visit, PMD parameters]</t>
+  </si>
+  <si>
+    <t>Biospecimen registrations by participant and visits</t>
+  </si>
+  <si>
+    <t>Every participant should have a registration for plasma and urine</t>
+  </si>
+  <si>
+    <t>provide examples; different plastic ware, sample mix up, sample lost, etc.</t>
+  </si>
+  <si>
+    <t>When the specimen is selected for shipment. You will be able to see the shipment information below and be able to indicate if a specimen was received.</t>
+  </si>
+  <si>
+    <t>If the specimen was shipped, the shipment information will be displayed here.</t>
+  </si>
+  <si>
+    <t>Mangement of the shipment of biospecimens</t>
+  </si>
+  <si>
     <t>Select the samples included in the shipment</t>
   </si>
   <si>
-    <t>Select the current status of the shipment</t>
-  </si>
-  <si>
-    <t>Enter the courier service</t>
-  </si>
-  <si>
-    <t>Enter the tracking number provided by the courier service</t>
-  </si>
-  <si>
-    <t>Enter the URL to the tracking page provided by the courier service</t>
-  </si>
-  <si>
-    <t>Enter the name of the person that is responsible for preparing and sending the shipment</t>
-  </si>
-  <si>
-    <t>Enter the date the shipment was sent</t>
-  </si>
-  <si>
-    <t>Select the origin point of the shipment</t>
-  </si>
-  <si>
-    <t>Select the destination point of the shipment</t>
-  </si>
-  <si>
-    <t>Enter the date the shipment was received at the destination point</t>
-  </si>
-  <si>
-    <t>Enter the name of the person that is responsible for receiving and unpacking the shipment</t>
-  </si>
-  <si>
-    <t>If applicable, enter additional information about the shipment</t>
-  </si>
-  <si>
-    <t>Select the participant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there whole genome or exome sequencing data of the participant in storage? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the previously generated sequencing data of the participant stored with a third party sequence provider, another healthcare provider or the site? </t>
-  </si>
-  <si>
-    <t>What is the name of the third party sequence provider?</t>
-  </si>
-  <si>
-    <t>Select the participant's disease status resulting from previous genetic testing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When was the genetic testing of this sequencing data performed (MM/YY)? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select from the list the sequencing system used? Only systems listed are accepted. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">What was the sequencing kit used? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the sequencing data previously generated been in the form of either FASTQs or CRAM files (in FASTA format), which encompass unmapped reads? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ftp secure transfer of sequencing data </t>
-  </si>
-  <si>
-    <t>Recon4IMD particpant identifier</t>
-  </si>
-  <si>
-    <t>Previous history of any surgery?</t>
-  </si>
-  <si>
-    <t>If yes, what surgery was performed and when did it occur?</t>
-  </si>
-  <si>
-    <t>Has the participant taken any medications or supplements in last 6 months?</t>
-  </si>
-  <si>
-    <t>Does the participant have any dietary restrictions or preferences?</t>
-  </si>
-  <si>
-    <t>What foods has the participant consumed within the last 24 hours?</t>
-  </si>
-  <si>
-    <t>When did the participant come off study?</t>
-  </si>
-  <si>
-    <t>Why is the participant coming off the study?</t>
-  </si>
-  <si>
-    <t>When a participant withdraws their consent, do they want their data used or deleted?</t>
-  </si>
-  <si>
-    <t>When a participant withdraws their consent, do they want their samples to be used, returned or destroyed?</t>
-  </si>
-  <si>
-    <t>If the patient has died, what is the date of death?</t>
-  </si>
-  <si>
-    <t>Participant identifier</t>
-  </si>
-  <si>
-    <t>Date of query</t>
-  </si>
-  <si>
-    <t>Reason for query</t>
-  </si>
-  <si>
-    <t>Sponsory query</t>
-  </si>
-  <si>
-    <t>Site response</t>
-  </si>
-  <si>
-    <t>Query identifier</t>
-  </si>
-  <si>
-    <t>IMD IEMbase</t>
-  </si>
-  <si>
-    <t>Prevalence data (number of patients) site specific (adult/pead)</t>
-  </si>
-  <si>
-    <t>Is the data correct (T/F)</t>
-  </si>
-  <si>
-    <t>If no, specify prevalence</t>
-  </si>
-  <si>
-    <t>Register new participants and manage existing registrations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select the Recon4IMD participant identifier. The Recon4IMD ID entered here should match that assigned to the participant during sampling and recorded on the related Biospecimen worksheet.   </t>
-  </si>
-  <si>
-    <t>Date the participant was entered into the IMDhub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select the participant's cohort assignment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants or legal representatives give written informed consent to study participation and consent for the collection and analysis of both blood and urine samples, and where indicated, a fibroblast sample or a stool sample. </t>
-  </si>
-  <si>
-    <t>Participant is suspected to have an IMD and was advised on genetic testing.</t>
-  </si>
-  <si>
-    <t>Particpant is informed of all the risks and benefits.</t>
-  </si>
-  <si>
-    <t>Participants enrolled or registered with one of the following participant registries or cohort study (with ethical approval at site): U-IMD, GENOMIT or Solve-RD.</t>
-  </si>
-  <si>
-    <t>If the participant is part of a participant registry or cohort study, select the registry.</t>
-  </si>
-  <si>
-    <t>Participants have the potential to be or a confirmed carrier of an IMD pathogenic variant.</t>
-  </si>
-  <si>
-    <t>E.g., cardiovascular, diabetes, hypertension, respiratory, gastrointestinal, nervous, urinary, endocrine, musculoskeletal, mental disorders, and addiction</t>
-  </si>
-  <si>
-    <t>E.g., HIV, infectious hepatitis, tuberculposis, or Creutzfeldt-Jakob disease</t>
-  </si>
-  <si>
-    <t>Participant had a blood transfusion within the last month</t>
-  </si>
-  <si>
-    <t>An indication that the participant meets selection criteria</t>
-  </si>
-  <si>
-    <t>An indication that the participant is confirmed with the registry</t>
-  </si>
-  <si>
-    <t>Registration of visits by participant and date</t>
-  </si>
-  <si>
-    <t>To generate the visit ID, please select a participant and the type of visit</t>
-  </si>
-  <si>
-    <t>Enter the Recon4IMD participant identifier. This identifier is generated upon participant registration into the IMDhub.</t>
-  </si>
-  <si>
-    <t>The enrollment visit is the initial study visit of the participant and the follow-up visit is any study visit after the initial study visit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fasting is when a subject doesn't eat or drink anything other than water only. </t>
-  </si>
-  <si>
-    <t>Comprised of the following clinical data fields: Demographics, Patient status, Disease history [IMD diagnosis including primary mitochondrial disease (PMD), Metabolites at diagnosis, Genetic results], Medical history [Family IMD history, Other conditions], Clinical exam, body weight and height at time of visit, Disease signs and symptoms at time of visit [Clinical progression, Human Phenotype Ontology, Neuropsychological testing, PMD symptoms, PMD brain imaging results], Treatment at time of visit [Drug Treatment, Dietary treatment, Renal therapy, Non-pharmacologic therapies], Laboratory analysis at time of visit [ERKNet parameters, Metabolites at visit, PMD parameters]</t>
-  </si>
-  <si>
-    <t>Biospecimen registrations by participant and visits</t>
-  </si>
-  <si>
-    <t>Every participant should have a registration for plasma and urine</t>
-  </si>
-  <si>
-    <t>provide examples; different plastic ware, sample mix up, sample lost, etc.</t>
-  </si>
-  <si>
-    <t>When the specimen is selected for shipment. You will be able to see the shipment information below and be able to indicate if a specimen was received.</t>
-  </si>
-  <si>
-    <t>If the specimen was shipped, the shipment information will be displayed here.</t>
-  </si>
-  <si>
-    <t>Mangement of the shipment of biospecimens</t>
-  </si>
-  <si>
     <t>Information on existing genetic data</t>
   </si>
   <si>
@@ -926,6 +935,9 @@
     <t>http://purl.obolibrary.org/obo/NCIT_C25426</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15220</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/OBI_0000810</t>
   </si>
   <si>
@@ -1220,6 +1232,9 @@
     <t>Participant cohorts</t>
   </si>
   <si>
+    <t>IEMbase diagnoses</t>
+  </si>
+  <si>
     <t>Consent for future research</t>
   </si>
   <si>
@@ -1238,6 +1253,9 @@
     <t>Shipment status</t>
   </si>
   <si>
+    <t>Shipment destinations</t>
+  </si>
+  <si>
     <t>Data storage owner types</t>
   </si>
   <si>
@@ -1277,6 +1295,9 @@
     <t>if (cohortAssignment === null) "Select the cohort that the participant is assigned to"</t>
   </si>
   <si>
+    <t>cohortAssignment !== null &amp;&amp; iembaseDiagnosis !== null ? (cohortAssignment.name.includes("Diagnosed IMD") ? "Select an IEMbase diagnosis" : false) : false</t>
+  </si>
+  <si>
     <t>if (hasGivenInformedConsent === null) "Indicate if the participant has given informed consent"</t>
   </si>
   <si>
@@ -1301,19 +1322,19 @@
     <t>if (hasAgreedToRecontactForFutureResearch === null) "Indicate if the participant has agreed to recontact for future research"</t>
   </si>
   <si>
-    <t>if (cohortAssignment.name === "Test cohort" &amp;&amp; hasAgreedToGeneticTesting == null) "Indicate if the participant has agreed to genetic testing"</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToGeneticAnalysis === null ? "Indicate if the participant has agreed to genetic analysis" : false ) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToTransferOfGeneticData === null ? "Indicate if the participant has agreed to the transfer of genetic data" : false ) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToRecontactOfMedicalFindings === null ? "Indicate if the participant has agreed to recontact in the event of medical findings" : false ) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (!cohortAssignment.name.includes("Negative") &amp;&amp; hasAgreedToRecontactOfIncidentalFindings === null ? "Indicate if the participant has agreed to recontact in the event of incidental findings" : false ) : false</t>
+    <t>if (cohortAssignment.definition === "positive control group" &amp;&amp; hasAgreedToGeneticTesting == null) "Indicate if the participant has agreed to genetic testing"</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.definition === "negative control cohort" &amp;&amp; hasAgreedToGeneticAnalysis === null ? "Indicate if the participant has agreed to genetic analysis" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.definition === "negative control cohort" &amp;&amp; hasAgreedToTransferOfGeneticData === null ? "Indicate if the participant has agreed to the transfer of genetic data" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.definition === "negative control cohort" &amp;&amp; hasAgreedToRecontactOfMedicalFindings === null ? "Indicate if the participant has agreed to recontact in the event of medical findings" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (!cohortAssignment.definition === "negative control cohort" &amp;&amp; hasAgreedToRecontactOfIncidentalFindings === null ? "Indicate if the participant has agreed to recontact in the event of incidental findings" : false ) : false</t>
   </si>
   <si>
     <t>if (hasRegistryAffiliation === null) "Indicate if the participant is part of an existing registry, cohort, or study"</t>
@@ -1325,19 +1346,19 @@
     <t>hasRegistryAffiliation &amp;&amp; participantDataRegistration !== null ? (participantRegistryIdentifier === null  &amp;&amp; participantDataRegistration.name !== "Not applicable" ? "Enter the participant's identifer that is used in that project" : false ) : false</t>
   </si>
   <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Negative control group (healthy)" &amp;&amp; isNotPotentialImd === null ? "Indicate if the particpant is or is not an potential IMD" : false ) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Negative control group (healthy)" &amp;&amp; hasNoHistoryOfImd === null ? "Indicate if the particpant has a history of IMDs" : false) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Negative control group (healthy)" &amp;&amp; hasNoHistoryOfMalignantTumors === null ? "Indicate if the particpant has a history of malignant tumors" : false) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Negative control group (healthy)" &amp;&amp; hasNoHistoryOfClinicalSystemicDiseases === null ? "Indicate if the particpant has a history of clinical systemic diseases" : false) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Negative control group (healthy)" &amp;&amp; hasNoHistoryOfInfectiousDiseases === null ? "Indicate if the participant has a history of infectious diseases" : false) : false</t>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" &amp;&amp; isNotPotentialImd === null ? "Indicate if the particpant is or is not an potential IMD" : false ) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" &amp;&amp; hasNoHistoryOfImd === null ? "Indicate if the particpant has a history of IMDs" : false) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" &amp;&amp; hasNoHistoryOfMalignantTumors === null ? "Indicate if the particpant has a history of malignant tumors" : false) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" &amp;&amp; hasNoHistoryOfClinicalSystemicDiseases === null ? "Indicate if the particpant has a history of clinical systemic diseases" : false) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" &amp;&amp; hasNoHistoryOfInfectiousDiseases === null ? "Indicate if the participant has a history of infectious diseases" : false) : false</t>
   </si>
   <si>
     <t>if (hasRegistryAffiliation &amp;&amp; hadNoRecentBloodTransfusion === null) "Indicate if the participant had no recent blood transfusion"</t>
@@ -1444,7 +1465,7 @@
     <t>if (dateShipmentCreated === null) "Enter the date the shipment was created"</t>
   </si>
   <si>
-    <t>if (!biospecimensShipped.length) "Select the samples that are included in this shipment"</t>
+    <t>if (biospecimensShipped === null) "Select the samples that are included in this shipment"</t>
   </si>
   <si>
     <t>if (shipmentStatus === null) "Select the current status of the shipment"</t>
@@ -1552,13 +1573,16 @@
     <t>if (sponsorQuery === null || sponsorQuery === "") "Please describe the query"</t>
   </si>
   <si>
+    <t>cohortAssignment !== null ? (cohortAssignment.name.includes("Diagnosed IMD") ? true : false) : false</t>
+  </si>
+  <si>
     <t>hasAgreedToFutureReuse</t>
   </si>
   <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Test cohort" ? true : false) : false</t>
-  </si>
-  <si>
-    <t>cohortAssignment !== null ? !cohortAssignment.name.includes("Negative") : false</t>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "positive control group" ? true : false) : false</t>
+  </si>
+  <si>
+    <t>cohortAssignment !== null ? !cohortAssignment.definition === "negative control cohort" : false</t>
   </si>
   <si>
     <t>hasRegistryAffiliation</t>
@@ -1567,7 +1591,7 @@
     <t>hasRegistryAffiliation &amp;&amp; participantDataRegistration</t>
   </si>
   <si>
-    <t>cohortAssignment !== null ? (cohortAssignment.name === "Negative control group (healthy)" ? true : false) : false</t>
+    <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" ? true : false) : false</t>
   </si>
   <si>
     <t>sexAtBirth !== null ? (sexAtBirth.name === "female" ? true : false) : false</t>
@@ -1579,7 +1603,7 @@
     <t>participantIsVerified !== null</t>
   </si>
   <si>
-    <t>FALSE</t>
+    <t>false</t>
   </si>
   <si>
     <t>specimenType !== null ? (["PAXgene-RNA", "EDTA-Blood/DNA"].includes(specimenType.name)) : false</t>
@@ -2025,7 +2049,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2089,16 +2113,16 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="P2" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q2" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2109,13 +2133,13 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P3" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q3" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2126,31 +2150,31 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H4" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="J4" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="L4" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="P4" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q4" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2161,28 +2185,28 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="I5" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J5" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="L5" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="P5" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q5" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2193,25 +2217,25 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="L6" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="P6" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q6" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2222,25 +2246,25 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="L7" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="O7" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="P7" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q7" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -2251,28 +2275,28 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="I8" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J8" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="L8" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="P8" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q8" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2283,28 +2307,28 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="I9" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J9" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="L9" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="P9" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q9" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2315,19 +2339,19 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="P10" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q10" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2338,31 +2362,31 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E11" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I11" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J11" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="L11" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="P11" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q11" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2373,19 +2397,31 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
+      </c>
+      <c r="I12" t="s">
+        <v>399</v>
+      </c>
+      <c r="J12" t="s">
+        <v>405</v>
+      </c>
+      <c r="L12" t="s">
+        <v>426</v>
+      </c>
+      <c r="M12" t="s">
+        <v>493</v>
       </c>
       <c r="P12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q12" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2396,25 +2432,19 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E13" t="s">
-        <v>260</v>
+        <v>162</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="L13" t="s">
-        <v>420</v>
+        <v>307</v>
       </c>
       <c r="P13" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q13" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -2425,22 +2455,25 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="E14" t="s">
+        <v>262</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="L14" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="P14" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q14" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2451,22 +2484,22 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="L15" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="P15" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q15" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2477,22 +2510,22 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="L16" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="P16" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q16" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2503,22 +2536,22 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="L17" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="P17" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q17" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2529,22 +2562,22 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="L18" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="P18" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q18" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2555,31 +2588,22 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="I19" t="s">
-        <v>395</v>
-      </c>
-      <c r="J19" t="s">
-        <v>401</v>
+        <v>313</v>
       </c>
       <c r="L19" t="s">
-        <v>426</v>
-      </c>
-      <c r="M19" t="s">
-        <v>486</v>
+        <v>432</v>
       </c>
       <c r="P19" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q19" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -2590,22 +2614,31 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
+      </c>
+      <c r="I20" t="s">
+        <v>399</v>
+      </c>
+      <c r="J20" t="s">
+        <v>406</v>
       </c>
       <c r="L20" t="s">
-        <v>427</v>
+        <v>433</v>
+      </c>
+      <c r="M20" t="s">
+        <v>494</v>
       </c>
       <c r="P20" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q20" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2616,28 +2649,22 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E21" t="s">
-        <v>261</v>
+        <v>170</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="L21" t="s">
-        <v>428</v>
-      </c>
-      <c r="M21" t="s">
-        <v>487</v>
+        <v>434</v>
       </c>
       <c r="P21" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q21" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -2648,28 +2675,28 @@
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="L22" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="M22" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="P22" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q22" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2680,25 +2707,28 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="E23" t="s">
+        <v>264</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="L23" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="M23" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="P23" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q23" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2709,25 +2739,25 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="L24" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="M24" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="P24" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q24" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2738,25 +2768,25 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="L25" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="M25" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="P25" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q25" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2767,16 +2797,25 @@
         <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="L26" t="s">
+        <v>439</v>
+      </c>
+      <c r="M26" t="s">
+        <v>496</v>
       </c>
       <c r="P26" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q26" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2787,25 +2826,16 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E27" t="s">
-        <v>263</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="L27" t="s">
-        <v>433</v>
+        <v>176</v>
       </c>
       <c r="P27" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q27" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2816,34 +2846,25 @@
         <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E28" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="I28" t="s">
-        <v>395</v>
-      </c>
-      <c r="J28" t="s">
-        <v>402</v>
+        <v>319</v>
       </c>
       <c r="L28" t="s">
-        <v>434</v>
-      </c>
-      <c r="M28" t="s">
-        <v>489</v>
+        <v>440</v>
       </c>
       <c r="P28" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q28" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2854,25 +2875,34 @@
         <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="E29" t="s">
+        <v>266</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
+      </c>
+      <c r="I29" t="s">
+        <v>399</v>
+      </c>
+      <c r="J29" t="s">
+        <v>407</v>
       </c>
       <c r="L29" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="M29" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="P29" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q29" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2883,16 +2913,25 @@
         <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="L30" t="s">
+        <v>442</v>
+      </c>
+      <c r="M30" t="s">
+        <v>498</v>
       </c>
       <c r="P30" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q30" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2903,28 +2942,16 @@
         <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D31" t="s">
-        <v>179</v>
-      </c>
-      <c r="E31" t="s">
-        <v>265</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="L31" t="s">
-        <v>436</v>
-      </c>
-      <c r="M31" t="s">
-        <v>491</v>
+        <v>180</v>
       </c>
       <c r="P31" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q31" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2935,25 +2962,28 @@
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="E32" t="s">
+        <v>267</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="L32" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="M32" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="P32" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q32" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2964,25 +2994,25 @@
         <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="L33" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="M33" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="P33" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q33" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2993,28 +3023,25 @@
         <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D34" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" t="s">
-        <v>266</v>
+        <v>183</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="L34" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="M34" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="P34" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q34" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -3025,28 +3052,28 @@
         <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="L35" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="M35" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="P35" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q35" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -3057,28 +3084,28 @@
         <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="L36" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="M36" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="P36" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q36" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="37" spans="1:17">
@@ -3089,22 +3116,28 @@
         <v>61</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D37" t="s">
-        <v>185</v>
+        <v>186</v>
+      </c>
+      <c r="E37" t="s">
+        <v>270</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="L37" t="s">
-        <v>442</v>
+        <v>448</v>
+      </c>
+      <c r="M37" t="s">
+        <v>497</v>
       </c>
       <c r="P37" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q37" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3115,25 +3148,22 @@
         <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="L38" t="s">
-        <v>443</v>
-      </c>
-      <c r="M38" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="P38" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q38" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="39" spans="1:17">
@@ -3144,19 +3174,25 @@
         <v>63</v>
       </c>
       <c r="C39" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D39" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
+      </c>
+      <c r="L39" t="s">
+        <v>450</v>
+      </c>
+      <c r="M39" t="s">
+        <v>500</v>
       </c>
       <c r="P39" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q39" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:17">
@@ -3167,25 +3203,19 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" t="s">
-        <v>269</v>
+        <v>139</v>
+      </c>
+      <c r="D40" t="s">
+        <v>189</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G40" t="s">
-        <v>393</v>
-      </c>
-      <c r="M40" t="s">
-        <v>493</v>
+        <v>329</v>
       </c>
       <c r="P40" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q40" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3196,77 +3226,68 @@
         <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E41" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
+      </c>
+      <c r="G41" t="s">
+        <v>397</v>
       </c>
       <c r="M41" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="P41" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q41" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>144</v>
       </c>
       <c r="E42" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
+      </c>
+      <c r="M42" t="s">
+        <v>502</v>
       </c>
       <c r="P42" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q42" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>18</v>
       </c>
-      <c r="B43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" t="s">
-        <v>188</v>
-      </c>
       <c r="E43" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="H43" t="s">
-        <v>394</v>
-      </c>
-      <c r="L43" t="s">
-        <v>444</v>
-      </c>
-      <c r="M43" t="s">
-        <v>495</v>
-      </c>
-      <c r="N43" t="s">
-        <v>512</v>
+        <v>332</v>
       </c>
       <c r="P43" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q43" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3277,28 +3298,34 @@
         <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D44" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="E44" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="J44" t="s">
-        <v>17</v>
+        <v>333</v>
+      </c>
+      <c r="H44" t="s">
+        <v>398</v>
       </c>
       <c r="L44" t="s">
-        <v>445</v>
+        <v>451</v>
+      </c>
+      <c r="M44" t="s">
+        <v>503</v>
+      </c>
+      <c r="N44" t="s">
+        <v>520</v>
       </c>
       <c r="P44" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q44" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3309,22 +3336,28 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" t="s">
-        <v>189</v>
+        <v>154</v>
+      </c>
+      <c r="E45" t="s">
+        <v>275</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>330</v>
+        <v>298</v>
+      </c>
+      <c r="J45" t="s">
+        <v>17</v>
       </c>
       <c r="L45" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="P45" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q45" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="46" spans="1:17">
@@ -3335,31 +3368,22 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" t="s">
-        <v>274</v>
+        <v>191</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="I46" t="s">
-        <v>395</v>
-      </c>
-      <c r="J46" t="s">
-        <v>403</v>
+        <v>334</v>
       </c>
       <c r="L46" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="P46" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q46" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="47" spans="1:17">
@@ -3370,25 +3394,31 @@
         <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D47" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E47" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
+      </c>
+      <c r="I47" t="s">
+        <v>399</v>
+      </c>
+      <c r="J47" t="s">
+        <v>408</v>
       </c>
       <c r="L47" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="P47" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q47" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -3399,22 +3429,25 @@
         <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="E48" t="s">
+        <v>277</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="L48" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="P48" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q48" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -3425,16 +3458,22 @@
         <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="D49" t="s">
+        <v>194</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
+      </c>
+      <c r="L49" t="s">
+        <v>456</v>
       </c>
       <c r="P49" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q49" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3448,19 +3487,13 @@
         <v>146</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="J50" t="s">
-        <v>19</v>
-      </c>
-      <c r="K50" t="s">
-        <v>82</v>
+        <v>338</v>
       </c>
       <c r="P50" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q50" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="51" spans="1:17">
@@ -3473,20 +3506,20 @@
       <c r="C51" t="s">
         <v>147</v>
       </c>
-      <c r="D51" t="s">
-        <v>193</v>
-      </c>
-      <c r="E51" t="s">
-        <v>276</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>335</v>
+        <v>297</v>
+      </c>
+      <c r="J51" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" t="s">
+        <v>83</v>
       </c>
       <c r="P51" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q51" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="52" spans="1:17">
@@ -3497,19 +3530,22 @@
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="D52" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="E52" t="s">
+        <v>278</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="P52" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q52" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -3520,56 +3556,59 @@
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="P53" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q53" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" t="s">
-        <v>277</v>
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" t="s">
+        <v>197</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>294</v>
+        <v>341</v>
       </c>
       <c r="P54" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q54" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>19</v>
       </c>
-      <c r="B55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>147</v>
+      <c r="E55" t="s">
+        <v>279</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="P55" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q55" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:17">
@@ -3580,25 +3619,16 @@
         <v>78</v>
       </c>
       <c r="C56" t="s">
-        <v>144</v>
-      </c>
-      <c r="D56" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="H56" t="s">
-        <v>394</v>
-      </c>
-      <c r="L56" t="s">
-        <v>450</v>
+        <v>297</v>
       </c>
       <c r="P56" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q56" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -3609,31 +3639,25 @@
         <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D57" t="s">
-        <v>197</v>
-      </c>
-      <c r="E57" t="s">
-        <v>278</v>
+        <v>198</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="I57" t="s">
-        <v>395</v>
-      </c>
-      <c r="J57" t="s">
-        <v>404</v>
+        <v>297</v>
+      </c>
+      <c r="H57" t="s">
+        <v>398</v>
       </c>
       <c r="L57" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="P57" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q57" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -3644,28 +3668,31 @@
         <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D58" t="s">
-        <v>198</v>
+        <v>199</v>
+      </c>
+      <c r="E58" t="s">
+        <v>280</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="M58" t="s">
-        <v>496</v>
-      </c>
-      <c r="N58" t="s">
-        <v>513</v>
-      </c>
-      <c r="O58" t="s">
-        <v>517</v>
+        <v>342</v>
+      </c>
+      <c r="I58" t="s">
+        <v>399</v>
+      </c>
+      <c r="J58" t="s">
+        <v>409</v>
+      </c>
+      <c r="L58" t="s">
+        <v>458</v>
       </c>
       <c r="P58" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q58" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="59" spans="1:17">
@@ -3676,28 +3703,28 @@
         <v>81</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D59" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="L59" t="s">
-        <v>452</v>
+        <v>343</v>
       </c>
       <c r="M59" t="s">
-        <v>497</v>
+        <v>504</v>
+      </c>
+      <c r="N59" t="s">
+        <v>521</v>
       </c>
       <c r="O59" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="P59" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q59" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -3708,25 +3735,28 @@
         <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D60" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="J60" t="s">
-        <v>18</v>
+        <v>344</v>
       </c>
       <c r="L60" t="s">
-        <v>453</v>
+        <v>459</v>
+      </c>
+      <c r="M60" t="s">
+        <v>505</v>
+      </c>
+      <c r="O60" t="s">
+        <v>526</v>
       </c>
       <c r="P60" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q60" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -3737,22 +3767,25 @@
         <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D61" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
+      </c>
+      <c r="J61" t="s">
+        <v>18</v>
       </c>
       <c r="L61" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="P61" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q61" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -3763,25 +3796,22 @@
         <v>84</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="L62" t="s">
-        <v>455</v>
-      </c>
-      <c r="M62" t="s">
-        <v>498</v>
+        <v>461</v>
       </c>
       <c r="P62" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q62" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -3792,25 +3822,25 @@
         <v>85</v>
       </c>
       <c r="C63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D63" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="L63" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="M63" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="P63" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q63" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -3821,31 +3851,25 @@
         <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="I64" t="s">
-        <v>395</v>
-      </c>
-      <c r="J64" t="s">
-        <v>405</v>
+        <v>348</v>
       </c>
       <c r="L64" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="M64" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="P64" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q64" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="65" spans="1:17">
@@ -3856,28 +3880,31 @@
         <v>87</v>
       </c>
       <c r="C65" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D65" t="s">
-        <v>205</v>
-      </c>
-      <c r="E65" t="s">
-        <v>279</v>
+        <v>206</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>343</v>
+        <v>349</v>
+      </c>
+      <c r="I65" t="s">
+        <v>399</v>
+      </c>
+      <c r="J65" t="s">
+        <v>410</v>
       </c>
       <c r="L65" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="M65" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="P65" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q65" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="66" spans="1:17">
@@ -3888,25 +3915,28 @@
         <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D66" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="E66" t="s">
+        <v>281</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="L66" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="M66" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="P66" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q66" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:17">
@@ -3917,25 +3947,25 @@
         <v>89</v>
       </c>
       <c r="C67" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D67" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="L67" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="M67" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="P67" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q67" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:17">
@@ -3946,19 +3976,25 @@
         <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
-      </c>
-      <c r="E68" t="s">
-        <v>280</v>
+        <v>146</v>
+      </c>
+      <c r="D68" t="s">
+        <v>209</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>347</v>
+        <v>350</v>
+      </c>
+      <c r="L68" t="s">
+        <v>467</v>
+      </c>
+      <c r="M68" t="s">
+        <v>510</v>
       </c>
       <c r="P68" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q68" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="69" spans="1:17">
@@ -3969,25 +4005,19 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E69" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="J69" t="s">
-        <v>20</v>
-      </c>
-      <c r="K69" t="s">
-        <v>97</v>
+        <v>351</v>
       </c>
       <c r="P69" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q69" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="70" spans="1:17">
@@ -3998,19 +4028,25 @@
         <v>92</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
-      </c>
-      <c r="D70" t="s">
-        <v>208</v>
+        <v>147</v>
+      </c>
+      <c r="E70" t="s">
+        <v>283</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
+      </c>
+      <c r="J70" t="s">
+        <v>20</v>
+      </c>
+      <c r="K70" t="s">
+        <v>98</v>
       </c>
       <c r="P70" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q70" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:17">
@@ -4021,31 +4057,19 @@
         <v>93</v>
       </c>
       <c r="C71" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D71" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="I71" t="s">
-        <v>395</v>
-      </c>
-      <c r="J71" t="s">
-        <v>406</v>
-      </c>
-      <c r="L71" t="s">
-        <v>461</v>
-      </c>
-      <c r="M71" t="s">
-        <v>503</v>
+        <v>352</v>
       </c>
       <c r="P71" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q71" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="72" spans="1:17">
@@ -4056,71 +4080,77 @@
         <v>94</v>
       </c>
       <c r="C72" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D72" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
+      </c>
+      <c r="I72" t="s">
+        <v>399</v>
+      </c>
+      <c r="J72" t="s">
+        <v>411</v>
       </c>
       <c r="L72" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="M72" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="P72" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q72" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" t="s">
-        <v>20</v>
-      </c>
-      <c r="E73" t="s">
-        <v>282</v>
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" t="s">
+        <v>146</v>
+      </c>
+      <c r="D73" t="s">
+        <v>212</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>347</v>
+        <v>353</v>
+      </c>
+      <c r="L73" t="s">
+        <v>469</v>
+      </c>
+      <c r="M73" t="s">
+        <v>512</v>
       </c>
       <c r="P73" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q73" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>20</v>
       </c>
-      <c r="B74" t="s">
-        <v>95</v>
-      </c>
-      <c r="C74" t="s">
-        <v>150</v>
-      </c>
-      <c r="D74" t="s">
-        <v>211</v>
+      <c r="E74" t="s">
+        <v>284</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="H74" t="s">
-        <v>394</v>
-      </c>
-      <c r="N74" t="s">
-        <v>514</v>
+        <v>351</v>
       </c>
       <c r="P74" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q74" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="75" spans="1:17">
@@ -4131,22 +4161,25 @@
         <v>96</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D75" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L75" t="s">
-        <v>463</v>
+        <v>354</v>
+      </c>
+      <c r="H75" t="s">
+        <v>398</v>
+      </c>
+      <c r="N75" t="s">
+        <v>522</v>
       </c>
       <c r="P75" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q75" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -4157,25 +4190,22 @@
         <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D76" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="J76" t="s">
-        <v>19</v>
+        <v>355</v>
       </c>
       <c r="L76" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="P76" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q76" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -4186,28 +4216,28 @@
         <v>98</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D77" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="E77" t="s">
+        <v>285</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="I77" t="s">
-        <v>395</v>
+        <v>297</v>
       </c>
       <c r="J77" t="s">
-        <v>406</v>
+        <v>19</v>
       </c>
       <c r="L77" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="P77" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q77" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -4218,19 +4248,28 @@
         <v>99</v>
       </c>
       <c r="C78" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D78" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
+      </c>
+      <c r="I78" t="s">
+        <v>399</v>
+      </c>
+      <c r="J78" t="s">
+        <v>411</v>
+      </c>
+      <c r="L78" t="s">
+        <v>472</v>
       </c>
       <c r="P78" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q78" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -4241,19 +4280,19 @@
         <v>100</v>
       </c>
       <c r="C79" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D79" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="P79" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q79" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4264,19 +4303,19 @@
         <v>101</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D80" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="P80" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q80" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="81" spans="1:17">
@@ -4287,19 +4326,19 @@
         <v>102</v>
       </c>
       <c r="C81" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D81" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="P81" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q81" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="82" spans="1:17">
@@ -4310,19 +4349,19 @@
         <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D82" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="P82" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q82" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="83" spans="1:17">
@@ -4333,28 +4372,19 @@
         <v>104</v>
       </c>
       <c r="C83" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D83" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="I83" t="s">
-        <v>395</v>
-      </c>
-      <c r="J83" t="s">
-        <v>397</v>
-      </c>
-      <c r="L83" t="s">
-        <v>466</v>
+        <v>360</v>
       </c>
       <c r="P83" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q83" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="84" spans="1:17">
@@ -4365,28 +4395,28 @@
         <v>105</v>
       </c>
       <c r="C84" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D84" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="I84" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J84" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="L84" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="P84" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q84" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="85" spans="1:17">
@@ -4400,16 +4430,25 @@
         <v>141</v>
       </c>
       <c r="D85" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
+      </c>
+      <c r="I85" t="s">
+        <v>399</v>
+      </c>
+      <c r="J85" t="s">
+        <v>412</v>
+      </c>
+      <c r="L85" t="s">
+        <v>474</v>
       </c>
       <c r="P85" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q85" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="86" spans="1:17">
@@ -4420,19 +4459,19 @@
         <v>107</v>
       </c>
       <c r="C86" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D86" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="P86" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q86" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:17">
@@ -4440,71 +4479,62 @@
         <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="C87" t="s">
         <v>145</v>
       </c>
       <c r="D87" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="P87" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q87" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:17">
       <c r="A88" t="s">
-        <v>21</v>
-      </c>
-      <c r="E88" t="s">
-        <v>283</v>
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" t="s">
+        <v>146</v>
+      </c>
+      <c r="D88" t="s">
+        <v>226</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="P88" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q88" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="89" spans="1:17">
       <c r="A89" t="s">
         <v>21</v>
       </c>
-      <c r="B89" t="s">
-        <v>67</v>
-      </c>
-      <c r="C89" t="s">
-        <v>139</v>
-      </c>
-      <c r="D89" t="s">
-        <v>225</v>
+      <c r="E89" t="s">
+        <v>286</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H89" t="s">
-        <v>394</v>
-      </c>
-      <c r="J89" t="s">
-        <v>17</v>
-      </c>
-      <c r="L89" t="s">
-        <v>468</v>
+        <v>366</v>
       </c>
       <c r="P89" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q89" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="90" spans="1:17">
@@ -4512,28 +4542,31 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="C90" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D90" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>363</v>
+        <v>298</v>
+      </c>
+      <c r="H90" t="s">
+        <v>398</v>
+      </c>
+      <c r="J90" t="s">
+        <v>17</v>
       </c>
       <c r="L90" t="s">
-        <v>469</v>
-      </c>
-      <c r="M90" t="s">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="P90" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q90" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -4544,31 +4577,25 @@
         <v>109</v>
       </c>
       <c r="C91" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D91" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="I91" t="s">
-        <v>395</v>
-      </c>
-      <c r="J91" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="L91" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="M91" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="P91" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q91" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="92" spans="1:17">
@@ -4579,25 +4606,31 @@
         <v>110</v>
       </c>
       <c r="C92" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D92" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
+      </c>
+      <c r="I92" t="s">
+        <v>399</v>
+      </c>
+      <c r="J92" t="s">
+        <v>413</v>
       </c>
       <c r="L92" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="M92" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="P92" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q92" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="93" spans="1:17">
@@ -4608,31 +4641,25 @@
         <v>111</v>
       </c>
       <c r="C93" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D93" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="I93" t="s">
-        <v>395</v>
-      </c>
-      <c r="J93" t="s">
-        <v>408</v>
+        <v>369</v>
       </c>
       <c r="L93" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="M93" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
       <c r="P93" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q93" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="94" spans="1:17">
@@ -4646,22 +4673,28 @@
         <v>141</v>
       </c>
       <c r="D94" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
+      </c>
+      <c r="I94" t="s">
+        <v>399</v>
+      </c>
+      <c r="J94" t="s">
+        <v>414</v>
       </c>
       <c r="L94" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="M94" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="P94" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q94" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="95" spans="1:17">
@@ -4672,31 +4705,25 @@
         <v>113</v>
       </c>
       <c r="C95" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D95" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="I95" t="s">
-        <v>395</v>
-      </c>
-      <c r="J95" t="s">
-        <v>409</v>
+        <v>371</v>
       </c>
       <c r="L95" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="M95" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="P95" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q95" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="96" spans="1:17">
@@ -4707,25 +4734,31 @@
         <v>114</v>
       </c>
       <c r="C96" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D96" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
+      </c>
+      <c r="I96" t="s">
+        <v>399</v>
+      </c>
+      <c r="J96" t="s">
+        <v>415</v>
       </c>
       <c r="L96" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="M96" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="P96" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q96" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="97" spans="1:17">
@@ -4736,25 +4769,25 @@
         <v>115</v>
       </c>
       <c r="C97" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D97" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="L97" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="M97" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="P97" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q97" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="98" spans="1:17">
@@ -4765,57 +4798,54 @@
         <v>116</v>
       </c>
       <c r="C98" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D98" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="L98" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="M98" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="P98" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q98" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="99" spans="1:17">
       <c r="A99" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B99" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="C99" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D99" t="s">
-        <v>235</v>
-      </c>
-      <c r="E99" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H99" t="s">
-        <v>394</v>
-      </c>
-      <c r="J99" t="s">
-        <v>17</v>
+        <v>375</v>
+      </c>
+      <c r="L99" t="s">
+        <v>484</v>
+      </c>
+      <c r="M99" t="s">
+        <v>517</v>
       </c>
       <c r="P99" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q99" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="100" spans="1:17">
@@ -4823,22 +4853,31 @@
         <v>22</v>
       </c>
       <c r="B100" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
       <c r="C100" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D100" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="E100" t="s">
+        <v>275</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>372</v>
+        <v>298</v>
+      </c>
+      <c r="H100" t="s">
+        <v>398</v>
+      </c>
+      <c r="J100" t="s">
+        <v>17</v>
       </c>
       <c r="P100" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q100" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="101" spans="1:17">
@@ -4849,19 +4888,19 @@
         <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D101" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="P101" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q101" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="102" spans="1:17">
@@ -4872,19 +4911,19 @@
         <v>119</v>
       </c>
       <c r="C102" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D102" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="P102" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q102" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="103" spans="1:17">
@@ -4895,19 +4934,19 @@
         <v>120</v>
       </c>
       <c r="C103" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D103" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="P103" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q103" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:17">
@@ -4918,68 +4957,59 @@
         <v>121</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D104" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="P104" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q104" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="105" spans="1:17">
       <c r="A105" t="s">
-        <v>23</v>
-      </c>
-      <c r="E105" t="s">
-        <v>284</v>
+        <v>22</v>
+      </c>
+      <c r="B105" t="s">
+        <v>122</v>
+      </c>
+      <c r="C105" t="s">
+        <v>145</v>
+      </c>
+      <c r="D105" t="s">
+        <v>242</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="P105" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q105" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="106" spans="1:17">
       <c r="A106" t="s">
         <v>23</v>
       </c>
-      <c r="B106" t="s">
-        <v>67</v>
-      </c>
-      <c r="C106" t="s">
-        <v>139</v>
-      </c>
-      <c r="D106" t="s">
-        <v>225</v>
+      <c r="E106" t="s">
+        <v>287</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H106" t="s">
-        <v>394</v>
-      </c>
-      <c r="J106" t="s">
-        <v>17</v>
-      </c>
-      <c r="L106" t="s">
-        <v>468</v>
+        <v>381</v>
       </c>
       <c r="P106" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q106" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="107" spans="1:17">
@@ -4987,25 +5017,31 @@
         <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="C107" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D107" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>378</v>
+        <v>298</v>
+      </c>
+      <c r="H107" t="s">
+        <v>398</v>
+      </c>
+      <c r="J107" t="s">
+        <v>17</v>
       </c>
       <c r="L107" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="P107" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q107" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="108" spans="1:17">
@@ -5016,28 +5052,22 @@
         <v>123</v>
       </c>
       <c r="C108" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D108" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="I108" t="s">
-        <v>395</v>
-      </c>
-      <c r="J108" t="s">
-        <v>410</v>
+        <v>382</v>
       </c>
       <c r="L108" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="P108" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q108" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="109" spans="1:17">
@@ -5048,31 +5078,28 @@
         <v>124</v>
       </c>
       <c r="C109" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D109" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="I109" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J109" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="L109" t="s">
-        <v>480</v>
-      </c>
-      <c r="M109" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="P109" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q109" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" spans="1:17">
@@ -5083,31 +5110,31 @@
         <v>125</v>
       </c>
       <c r="C110" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D110" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="I110" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J110" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="L110" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="M110" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="P110" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q110" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="111" spans="1:17">
@@ -5121,71 +5148,74 @@
         <v>141</v>
       </c>
       <c r="D111" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
+      </c>
+      <c r="I111" t="s">
+        <v>399</v>
+      </c>
+      <c r="J111" t="s">
+        <v>418</v>
       </c>
       <c r="L111" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="M111" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="P111" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q111" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="112" spans="1:17">
       <c r="A112" t="s">
-        <v>24</v>
-      </c>
-      <c r="E112" t="s">
-        <v>285</v>
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>127</v>
+      </c>
+      <c r="C112" t="s">
+        <v>142</v>
+      </c>
+      <c r="D112" t="s">
+        <v>247</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>383</v>
+        <v>386</v>
+      </c>
+      <c r="L112" t="s">
+        <v>489</v>
+      </c>
+      <c r="M112" t="s">
+        <v>519</v>
       </c>
       <c r="P112" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q112" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="113" spans="1:17">
       <c r="A113" t="s">
         <v>24</v>
       </c>
-      <c r="B113" t="s">
-        <v>67</v>
-      </c>
-      <c r="C113" t="s">
-        <v>139</v>
-      </c>
-      <c r="D113" t="s">
-        <v>246</v>
-      </c>
       <c r="E113" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="J113" t="s">
-        <v>17</v>
-      </c>
-      <c r="L113" t="s">
-        <v>468</v>
+        <v>387</v>
       </c>
       <c r="P113" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q113" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="114" spans="1:17">
@@ -5193,28 +5223,31 @@
         <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>127</v>
+        <v>68</v>
       </c>
       <c r="C114" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D114" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E114" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>351</v>
+        <v>298</v>
+      </c>
+      <c r="J114" t="s">
+        <v>17</v>
       </c>
       <c r="L114" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="P114" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q114" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="115" spans="1:17">
@@ -5225,25 +5258,25 @@
         <v>128</v>
       </c>
       <c r="C115" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D115" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E115" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="L115" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="P115" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q115" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -5257,22 +5290,22 @@
         <v>145</v>
       </c>
       <c r="D116" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E116" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="L116" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="P116" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q116" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="117" spans="1:17">
@@ -5283,22 +5316,25 @@
         <v>130</v>
       </c>
       <c r="C117" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D117" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E117" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
+      </c>
+      <c r="L117" t="s">
+        <v>492</v>
       </c>
       <c r="P117" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q117" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="118" spans="1:17">
@@ -5309,71 +5345,71 @@
         <v>131</v>
       </c>
       <c r="C118" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D118" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E118" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="H118" t="s">
-        <v>394</v>
-      </c>
-      <c r="N118" t="s">
-        <v>515</v>
+        <v>390</v>
       </c>
       <c r="P118" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q118" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="119" spans="1:17">
       <c r="A119" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B119" t="s">
+        <v>132</v>
+      </c>
+      <c r="C119" t="s">
+        <v>151</v>
+      </c>
+      <c r="D119" t="s">
+        <v>253</v>
       </c>
       <c r="E119" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
+      </c>
+      <c r="H119" t="s">
+        <v>398</v>
+      </c>
+      <c r="N119" t="s">
+        <v>523</v>
       </c>
       <c r="P119" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q119" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="120" spans="1:17">
       <c r="A120" t="s">
         <v>25</v>
       </c>
-      <c r="B120" t="s">
-        <v>132</v>
-      </c>
-      <c r="C120" t="s">
-        <v>144</v>
-      </c>
-      <c r="D120" t="s">
-        <v>252</v>
+      <c r="E120" t="s">
+        <v>295</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="H120" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="P120" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q120" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="121" spans="1:17">
@@ -5384,19 +5420,22 @@
         <v>133</v>
       </c>
       <c r="C121" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D121" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>389</v>
+        <v>322</v>
+      </c>
+      <c r="H121" t="s">
+        <v>398</v>
       </c>
       <c r="P121" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q121" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -5410,16 +5449,16 @@
         <v>143</v>
       </c>
       <c r="D122" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="P122" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q122" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -5433,56 +5472,56 @@
         <v>144</v>
       </c>
       <c r="D123" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="P123" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q123" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="124" spans="1:17">
       <c r="A124" t="s">
-        <v>26</v>
-      </c>
-      <c r="E124" t="s">
-        <v>293</v>
+        <v>25</v>
+      </c>
+      <c r="B124" t="s">
+        <v>136</v>
+      </c>
+      <c r="C124" t="s">
+        <v>145</v>
+      </c>
+      <c r="D124" t="s">
+        <v>257</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="P124" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q124" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="125" spans="1:17">
       <c r="A125" t="s">
         <v>26</v>
       </c>
-      <c r="B125" t="s">
-        <v>136</v>
-      </c>
-      <c r="C125" t="s">
-        <v>136</v>
+      <c r="E125" t="s">
+        <v>296</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="H125" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="P125" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q125" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="1:17">
@@ -5493,16 +5532,39 @@
         <v>137</v>
       </c>
       <c r="C126" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>361</v>
+        <v>396</v>
+      </c>
+      <c r="H126" t="s">
+        <v>398</v>
       </c>
       <c r="P126" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="Q126" t="s">
-        <v>393</v>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17">
+      <c r="A127" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" t="s">
+        <v>138</v>
+      </c>
+      <c r="C127" t="s">
+        <v>146</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="P127" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -5530,10 +5592,10 @@
     <hyperlink ref="F23" r:id="rId21"/>
     <hyperlink ref="F24" r:id="rId22"/>
     <hyperlink ref="F25" r:id="rId23"/>
-    <hyperlink ref="F27" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId24"/>
     <hyperlink ref="F28" r:id="rId25"/>
     <hyperlink ref="F29" r:id="rId26"/>
-    <hyperlink ref="F31" r:id="rId27"/>
+    <hyperlink ref="F30" r:id="rId27"/>
     <hyperlink ref="F32" r:id="rId28"/>
     <hyperlink ref="F33" r:id="rId29"/>
     <hyperlink ref="F34" r:id="rId30"/>
@@ -5589,8 +5651,8 @@
     <hyperlink ref="F84" r:id="rId80"/>
     <hyperlink ref="F85" r:id="rId81"/>
     <hyperlink ref="F86" r:id="rId82"/>
-    <hyperlink ref="F87" r:id="rId83" location="comment"/>
-    <hyperlink ref="F88" r:id="rId84"/>
+    <hyperlink ref="F87" r:id="rId83"/>
+    <hyperlink ref="F88" r:id="rId84" location="comment"/>
     <hyperlink ref="F89" r:id="rId85"/>
     <hyperlink ref="F90" r:id="rId86"/>
     <hyperlink ref="F91" r:id="rId87"/>
@@ -5628,7 +5690,8 @@
     <hyperlink ref="F123" r:id="rId119"/>
     <hyperlink ref="F124" r:id="rId120"/>
     <hyperlink ref="F125" r:id="rId121"/>
-    <hyperlink ref="F126" r:id="rId122" location="comment"/>
+    <hyperlink ref="F126" r:id="rId122"/>
+    <hyperlink ref="F127" r:id="rId123" location="comment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: changed 'sex at birth' to 'gender at birth'
</commit_message>
<xml_diff>
--- a/files/imdhub-site.xlsx
+++ b/files/imdhub-site.xlsx
@@ -115,7 +115,7 @@
     <t>month of birth</t>
   </si>
   <si>
-    <t>sex at birth</t>
+    <t>gender at birth</t>
   </si>
   <si>
     <t>study criteria</t>
@@ -1313,7 +1313,7 @@
     <t>if (monthOfBirth === null) "Enter the month the participant was born"</t>
   </si>
   <si>
-    <t>if (sexAtBirth === null) "Select the sex of the participant"</t>
+    <t>if (genderAtBirth === null) "Select the sex of the participant"</t>
   </si>
   <si>
     <t>if (cohortAssignment === null) "Select the cohort that the participant is assigned to"</t>
@@ -1394,7 +1394,7 @@
     <t>if (hadNoRecentHaemodialysis === null) "Indicate if the participant had no recent haemodialysis"</t>
   </si>
   <si>
-    <t>sexAtBirth !== null ? (sexAtBirth.name === "female" &amp;&amp; participantIsNotPregnantOrLactating == null ? "Indicate if the participant is pregnant or lacting" : false) : false</t>
+    <t>genderAtBirth !== null ? (genderAtBirth.name === "female" &amp;&amp; participantIsNotPregnantOrLactating == null ? "Indicate if the participant is pregnant or lacting" : false) : false</t>
   </si>
   <si>
     <t>if (visitId === null) "To generate the visit ID, select a participant and specify the visit type"</t>
@@ -1618,7 +1618,7 @@
     <t>cohortAssignment !== null ? (cohortAssignment.definition === "negative control cohort" ? true : false) : false</t>
   </si>
   <si>
-    <t>sexAtBirth !== null ? (sexAtBirth.name === "female" ? true : false) : false</t>
+    <t>genderAtBirth !== null ? (genderAtBirth.name === "female" ? true : false) : false</t>
   </si>
   <si>
     <t>participantIsEligible !== null</t>

</xml_diff>